<commit_message>
Fixed Test & Added Wishlist 2 Tests
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="223">
   <si>
     <t>P_Key</t>
   </si>
@@ -693,12 +693,16 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -781,7 +785,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,6 +813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,7 +911,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,9 +968,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -971,10 +978,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1379,7 +1390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1395,18 +1406,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1773,22 +1784,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="99" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="3.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="4.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="10" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1867,7 +1878,9 @@
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9">
@@ -1892,7 +1905,9 @@
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9">
@@ -1917,11 +1932,13 @@
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1967,7 +1984,9 @@
       <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9">
@@ -1992,7 +2011,9 @@
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9">
@@ -2042,7 +2063,9 @@
       <c r="G10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9">
@@ -2067,7 +2090,9 @@
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9">
@@ -2092,7 +2117,9 @@
       <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9">
@@ -2167,7 +2194,9 @@
       <c r="G15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9">
@@ -2221,7 +2250,7 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="33" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2248,7 +2277,7 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -2269,7 +2298,9 @@
       <c r="G19" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9">
@@ -2288,7 +2319,7 @@
       <c r="E20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="34" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -2313,7 +2344,7 @@
       <c r="E21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="34" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -2326,10 +2357,10 @@
       <c r="A22" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>199</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2338,7 +2369,7 @@
       <c r="E22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="34" t="s">
         <v>200</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -2363,13 +2394,15 @@
       <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="35" t="s">
         <v>172</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9">
@@ -2388,13 +2421,15 @@
       <c r="E24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="35" t="s">
         <v>174</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9">
@@ -2413,13 +2448,15 @@
       <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="35" t="s">
         <v>179</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9">
@@ -2438,7 +2475,7 @@
       <c r="E26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="35" t="s">
         <v>175</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -2454,7 +2491,7 @@
       <c r="B27" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -2463,7 +2500,7 @@
       <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="34" t="s">
         <v>215</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -2479,7 +2516,7 @@
       <c r="B28" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2488,7 +2525,7 @@
       <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="34" t="s">
         <v>216</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -2504,7 +2541,7 @@
       <c r="B29" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2513,7 +2550,7 @@
       <c r="E29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="34" t="s">
         <v>216</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -2529,7 +2566,7 @@
       <c r="B30" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2538,7 +2575,7 @@
       <c r="E30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="34" t="s">
         <v>217</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -2554,7 +2591,7 @@
       <c r="B31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2563,7 +2600,7 @@
       <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="34" t="s">
         <v>218</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -2579,7 +2616,7 @@
       <c r="B32" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="32" t="s">
         <v>208</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2588,7 +2625,7 @@
       <c r="E32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="34" t="s">
         <v>219</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -2619,17 +2656,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2792,13 +2829,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="8" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3169,14 +3206,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3273,11 +3310,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3343,11 +3380,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3413,10 +3450,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3449,7 +3486,7 @@
       <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>171</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -3475,7 +3512,7 @@
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="24" t="s">
@@ -3501,7 +3538,7 @@
       <c r="A4" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>176</v>
       </c>
       <c r="C4" s="24" t="s">
@@ -3527,7 +3564,7 @@
       <c r="A5" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>177</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -3566,11 +3603,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
1. Fixed some defects and ran all together 2. Marked the incomplete test cases in yellow.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testcrew Projects\Jahez\CrewCentricFeb2022ProjectSuite\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CCAAD3-8EEE-43FC-8652-B6EB06ACEC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5351F0-D0DB-4C03-8F7F-BADC5DDAF115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
   <si>
     <t>P_Key</t>
   </si>
@@ -714,16 +714,12 @@
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -843,14 +839,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -932,7 +928,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,9 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -975,8 +968,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -987,7 +978,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -999,83 +990,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{6F6F5C68-DDD5-4CC2-8A19-08616A0C669A}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <fill>
         <patternFill>
@@ -1381,22 +1315,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB359C22-D3C7-4FE1-8608-AABCC891EBD5}" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB359C22-D3C7-4FE1-8608-AABCC891EBD5}" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A5:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ACFED27A-644C-4D99-B969-D745294BCC0C}" name="WebConfiguration" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{DF6E5BE3-671C-4C60-ABB0-3753BEEBFAF5}" name="BaseURL" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{FFC07966-A6BC-4B72-8C02-E5C51BFAFAE7}" name="Browser" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{9E6EB733-62C2-4706-B265-040C82226523}" name="Width" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{A4FE3405-ADAD-46C4-9513-5742581DCB44}" name="Height" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{3E988624-98D4-4949-808D-0C0044CC74F2}" name="MAXWait" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{ACFED27A-644C-4D99-B969-D745294BCC0C}" name="WebConfiguration" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{DF6E5BE3-671C-4C60-ABB0-3753BEEBFAF5}" name="BaseURL" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{FFC07966-A6BC-4B72-8C02-E5C51BFAFAE7}" name="Browser" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{9E6EB733-62C2-4706-B265-040C82226523}" name="Width" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{A4FE3405-ADAD-46C4-9513-5742581DCB44}" name="Height" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{3E988624-98D4-4949-808D-0C0044CC74F2}" name="MAXWait" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A202B514-692E-43D7-80EE-CF59B102E858}" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A202B514-692E-43D7-80EE-CF59B102E858}" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="A13:N19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{04B81B3A-BDC1-4FED-B2F4-FC472A65C019}" name="MobileConfiguration"/>
@@ -1407,10 +1341,10 @@
     <tableColumn id="6" xr3:uid="{1EAA9812-0829-4B31-8029-D644E94161FD}" name="AppName"/>
     <tableColumn id="12" xr3:uid="{F308F5CB-C8D3-4526-B813-845DE4B9ACAE}" name="AppURL"/>
     <tableColumn id="7" xr3:uid="{4839977E-FA2C-4469-BCF1-5773FE2944F3}" name="AppPackage"/>
-    <tableColumn id="8" xr3:uid="{DD89DEF0-FBCE-40CB-8F12-5FA050EA85BE}" name="AppActivity" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{DD89DEF0-FBCE-40CB-8F12-5FA050EA85BE}" name="AppActivity" dataDxfId="32"/>
     <tableColumn id="9" xr3:uid="{049B6ADF-10BA-47F2-98E2-7CB770EA658C}" name="AppiumURL"/>
     <tableColumn id="10" xr3:uid="{6DFFC595-F307-4F65-9FE7-2512A6A0DFE6}" name="AutomationName"/>
-    <tableColumn id="11" xr3:uid="{508B4E97-D822-4A53-B936-59EA04B1700F}" name="AutoGrantPermissions" dataDxfId="41"/>
+    <tableColumn id="11" xr3:uid="{508B4E97-D822-4A53-B936-59EA04B1700F}" name="AutoGrantPermissions" dataDxfId="31"/>
     <tableColumn id="13" xr3:uid="{5F245076-7D13-45BE-BF42-6266EDAE5F30}" name="Project"/>
     <tableColumn id="14" xr3:uid="{C7E05931-4C98-4596-B9E9-587BCB3A8628}" name="Build"/>
   </tableColumns>
@@ -1422,7 +1356,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{23F08F6A-37D2-4B28-B4C1-F398833727B3}" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{38F71438-F73C-4EAB-A991-8F932EB83E04}" name="Platform" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{38F71438-F73C-4EAB-A991-8F932EB83E04}" name="Platform" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{FA881134-7F69-4127-B06D-F7EBFEB0C12B}" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1700,18 +1634,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="40.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="39.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="80.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="46.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="80.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1726,18 +1660,18 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
@@ -1765,102 +1699,102 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <v>1920</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>1080</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="19">
         <v>5</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="19">
         <v>1920</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>1080</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="19">
         <v>5</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>1080</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>1080</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="19">
         <v>5</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
@@ -1878,7 +1812,7 @@
       <c r="E13" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="21" t="s">
         <v>148</v>
       </c>
       <c r="G13" t="s">
@@ -1890,7 +1824,7 @@
       <c r="I13" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="21" t="s">
         <v>152</v>
       </c>
       <c r="K13" t="s">
@@ -1930,13 +1864,13 @@
       <c r="B15" t="s">
         <v>161</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="30">
         <v>11</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="23" t="s">
         <v>163</v>
       </c>
       <c r="F15" t="s">
@@ -1948,13 +1882,13 @@
       <c r="I15" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="24" t="s">
         <v>167</v>
       </c>
       <c r="K15" t="s">
         <v>168</v>
       </c>
-      <c r="L15" s="28" t="s">
+      <c r="L15" s="25" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1965,13 +1899,13 @@
       <c r="B16" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="23" t="s">
         <v>176</v>
       </c>
       <c r="F16" t="s">
@@ -1983,13 +1917,13 @@
       <c r="I16" t="s">
         <v>166</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="24" t="s">
         <v>167</v>
       </c>
       <c r="K16" t="s">
         <v>168</v>
       </c>
-      <c r="L16" s="28" t="s">
+      <c r="L16" s="25" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2000,13 +1934,13 @@
       <c r="B17" t="s">
         <v>174</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="23" t="s">
         <v>172</v>
       </c>
       <c r="F17" t="s">
@@ -2021,19 +1955,19 @@
       <c r="I17" t="s">
         <v>166</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="28" t="s">
         <v>178</v>
       </c>
       <c r="K17" t="s">
         <v>168</v>
       </c>
-      <c r="L17" s="28" t="s">
+      <c r="L17" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="M17" s="27" t="s">
+      <c r="M17" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="N17" s="27" t="s">
+      <c r="N17" s="24" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2044,7 +1978,7 @@
       <c r="B18" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="29" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2052,7 +1986,7 @@
       <c r="A19" t="s">
         <v>183</v>
       </c>
-      <c r="E19" s="26"/>
+      <c r="E19" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2077,21 +2011,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="92.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="7.44140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.21875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2137,29 +2071,29 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
@@ -2168,7 +2102,7 @@
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2177,11 +2111,11 @@
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>227</v>
+      <c r="G4" s="31" t="s">
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
@@ -2195,7 +2129,7 @@
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2204,11 +2138,11 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>227</v>
+      <c r="G5" s="31" t="s">
+        <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>14</v>
@@ -2244,39 +2178,41 @@
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1">
+      <c r="A8" s="31">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
@@ -2294,13 +2230,15 @@
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9">
@@ -2319,39 +2257,41 @@
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="1">
+      <c r="A11" s="31">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
@@ -2369,13 +2309,15 @@
       <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
@@ -2394,13 +2336,15 @@
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
@@ -2419,89 +2363,91 @@
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="1">
+      <c r="A15" s="31">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="1">
+      <c r="A16" s="31">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1">
+      <c r="A17" s="31">
         <v>14</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
@@ -2519,39 +2465,41 @@
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1">
+      <c r="A19" s="31">
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="9"/>
@@ -2582,10 +2530,10 @@
       <c r="E21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -2609,10 +2557,10 @@
       <c r="E22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="2"/>
@@ -2632,56 +2580,56 @@
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="1">
+      <c r="A24" s="31">
         <v>19</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1">
+      <c r="A25" s="31">
         <v>20</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9"/>
@@ -2697,31 +2645,31 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="1">
+      <c r="A27" s="31">
         <v>21</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="2"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9"/>
@@ -2743,7 +2691,7 @@
       <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2752,13 +2700,15 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9">
@@ -2768,7 +2718,7 @@
       <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2777,13 +2727,15 @@
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9">
@@ -2793,7 +2745,7 @@
       <c r="B31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2802,39 +2754,41 @@
       <c r="E31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="1">
+      <c r="A32" s="31">
         <v>25</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="9"/>
@@ -2850,294 +2804,262 @@
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="1">
+      <c r="A34" s="31">
         <v>26</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="1">
+      <c r="A35" s="31">
         <v>27</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="1">
+      <c r="A36" s="31">
         <v>28</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="1">
+      <c r="A37" s="31">
         <v>29</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="1">
+      <c r="A38" s="31">
         <v>30</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G38" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="1">
+      <c r="A39" s="31">
         <v>31</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G1:G3 G6:G7 G10:G11 G14 G23:G25 G28:G32 G40:G1048576">
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+  <conditionalFormatting sqref="G11 G23:G25 G40:G1048576 G1:G7 G28:G32">
+    <cfRule type="cellIs" dxfId="29" priority="53" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20 G22:G25">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G25">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G39">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
+  <conditionalFormatting sqref="G17:G18">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9:G10">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -3145,7 +3067,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="G12:G14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
@@ -3176,17 +3098,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5546875" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3343,18 +3265,18 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.21875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="8" max="10" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3718,8 +3640,12 @@
       <c r="D13" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -3761,14 +3687,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3865,11 +3791,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3937,11 +3863,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3994,10 +3920,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="6" max="8" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4146,11 +4072,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.21875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Temp commit & Extent Report Logo Added
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testcrew Projects\Jahez\CrewCentricFeb2022ProjectSuite\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5351F0-D0DB-4C03-8F7F-BADC5DDAF115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -23,9 +17,9 @@
     <sheet name="CustomerPayments" sheetId="17" r:id="rId8"/>
     <sheet name="HomePage" sheetId="18" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="228">
   <si>
     <t>P_Key</t>
   </si>
@@ -714,12 +708,16 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -1006,7 +1004,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{6F6F5C68-DDD5-4CC2-8A19-08616A0C669A}"/>
+    <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
@@ -1227,7 +1225,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1264,25 +1262,25 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1315,49 +1313,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB359C22-D3C7-4FE1-8608-AABCC891EBD5}" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A5:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A5:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ACFED27A-644C-4D99-B969-D745294BCC0C}" name="WebConfiguration" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{DF6E5BE3-671C-4C60-ABB0-3753BEEBFAF5}" name="BaseURL" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{FFC07966-A6BC-4B72-8C02-E5C51BFAFAE7}" name="Browser" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{9E6EB733-62C2-4706-B265-040C82226523}" name="Width" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{A4FE3405-ADAD-46C4-9513-5742581DCB44}" name="Height" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{3E988624-98D4-4949-808D-0C0044CC74F2}" name="MAXWait" dataDxfId="34"/>
+    <tableColumn id="1" name="WebConfiguration" dataDxfId="39"/>
+    <tableColumn id="2" name="BaseURL" dataDxfId="38"/>
+    <tableColumn id="3" name="Browser" dataDxfId="37"/>
+    <tableColumn id="4" name="Width" dataDxfId="36"/>
+    <tableColumn id="5" name="Height" dataDxfId="35"/>
+    <tableColumn id="6" name="MAXWait" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A202B514-692E-43D7-80EE-CF59B102E858}" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="33">
-  <autoFilter ref="A13:N19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="33">
+  <autoFilter ref="A13:N19"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{04B81B3A-BDC1-4FED-B2F4-FC472A65C019}" name="MobileConfiguration"/>
-    <tableColumn id="2" xr3:uid="{18CC430D-B773-470D-B9B4-847CDF42C429}" name="DeviceType"/>
-    <tableColumn id="3" xr3:uid="{3E558CA4-250B-4A17-B20F-9619D37D1466}" name="PlatformName"/>
-    <tableColumn id="4" xr3:uid="{513E123B-E4BB-4634-AF8B-9BBC3C4E66FC}" name="Version"/>
-    <tableColumn id="5" xr3:uid="{832229A9-5488-4DA6-A654-CA56D906E3E6}" name="DeviceName"/>
-    <tableColumn id="6" xr3:uid="{1EAA9812-0829-4B31-8029-D644E94161FD}" name="AppName"/>
-    <tableColumn id="12" xr3:uid="{F308F5CB-C8D3-4526-B813-845DE4B9ACAE}" name="AppURL"/>
-    <tableColumn id="7" xr3:uid="{4839977E-FA2C-4469-BCF1-5773FE2944F3}" name="AppPackage"/>
-    <tableColumn id="8" xr3:uid="{DD89DEF0-FBCE-40CB-8F12-5FA050EA85BE}" name="AppActivity" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{049B6ADF-10BA-47F2-98E2-7CB770EA658C}" name="AppiumURL"/>
-    <tableColumn id="10" xr3:uid="{6DFFC595-F307-4F65-9FE7-2512A6A0DFE6}" name="AutomationName"/>
-    <tableColumn id="11" xr3:uid="{508B4E97-D822-4A53-B936-59EA04B1700F}" name="AutoGrantPermissions" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{5F245076-7D13-45BE-BF42-6266EDAE5F30}" name="Project"/>
-    <tableColumn id="14" xr3:uid="{C7E05931-4C98-4596-B9E9-587BCB3A8628}" name="Build"/>
+    <tableColumn id="1" name="MobileConfiguration"/>
+    <tableColumn id="2" name="DeviceType"/>
+    <tableColumn id="3" name="PlatformName"/>
+    <tableColumn id="4" name="Version"/>
+    <tableColumn id="5" name="DeviceName"/>
+    <tableColumn id="6" name="AppName"/>
+    <tableColumn id="12" name="AppURL"/>
+    <tableColumn id="7" name="AppPackage"/>
+    <tableColumn id="8" name="AppActivity" dataDxfId="32"/>
+    <tableColumn id="9" name="AppiumURL"/>
+    <tableColumn id="10" name="AutomationName"/>
+    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="31"/>
+    <tableColumn id="13" name="Project"/>
+    <tableColumn id="14" name="Build"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{23F08F6A-37D2-4B28-B4C1-F398833727B3}" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{38F71438-F73C-4EAB-A991-8F932EB83E04}" name="Platform" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{FA881134-7F69-4127-B06D-F7EBFEB0C12B}" name="Reference"/>
+    <tableColumn id="1" name="Platform" dataDxfId="30"/>
+    <tableColumn id="2" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1406,7 +1404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1441,7 +1439,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1625,27 +1623,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6E12C0-EB29-4989-BDD1-D7BB74957C32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="46.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="80.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1990,12 +1988,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15" xr:uid="{00679324-331A-4AE2-AE2D-1F79565327E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J17" r:id="rId1" xr:uid="{0B094444-006F-471E-97DD-339A11C7A1E9}"/>
+    <hyperlink ref="J17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2008,24 +2006,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.44140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="92.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="7.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2599,7 +2597,7 @@
         <v>70</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="H24" s="32" t="s">
         <v>14</v>
@@ -3076,10 +3074,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H39">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>"Web,Api,Web-Api,Mobile"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3089,26 +3087,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48812811-E93A-46F9-8282-4F2691629E6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3253,7 +3251,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{B80FD0FC-F01E-4E90-BED4-4DE8FDF551A8}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3261,22 +3259,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A124E-D40D-4A93-830F-790EB33FE49D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="8" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3678,23 +3676,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A6C346-A076-40B3-B7FC-7E5C01E71FCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3782,20 +3780,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713FD22A-9E27-4A0B-8E5D-03C18E5FFC26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3854,20 +3852,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCE8493-E501-4D12-A2CC-249AD4238AF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3911,19 +3909,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E452DD-0920-4621-B1C6-EC97052614E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="6" max="8" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4063,20 +4061,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21322546-F485-4C46-8AE3-96F6F7CAA90C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Home Page Test & Address Test Added, Assertions Added & Refactor code inprogress.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
     <sheet name="Controller" sheetId="1" r:id="rId2"/>
     <sheet name="RegistrationAndLogin" sheetId="12" r:id="rId3"/>
-    <sheet name="CartAndCheckout" sheetId="13" r:id="rId4"/>
-    <sheet name="Wishlist" sheetId="14" r:id="rId5"/>
-    <sheet name="MyAddresses" sheetId="15" r:id="rId6"/>
+    <sheet name="Wishlist" sheetId="14" r:id="rId4"/>
+    <sheet name="MyAddresses" sheetId="15" r:id="rId5"/>
+    <sheet name="HomePage" sheetId="18" r:id="rId6"/>
     <sheet name="ChangePassword" sheetId="16" r:id="rId7"/>
-    <sheet name="CustomerPayments" sheetId="17" r:id="rId8"/>
-    <sheet name="HomePage" sheetId="18" r:id="rId9"/>
+    <sheet name="CartAndCheckout" sheetId="13" r:id="rId8"/>
+    <sheet name="CustomerPayments" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="241">
   <si>
     <t>P_Key</t>
   </si>
@@ -605,15 +605,9 @@
     <t>EMPTY</t>
   </si>
   <si>
-    <t>PIK10</t>
-  </si>
-  <si>
     <t>PIK10@gmail.com</t>
   </si>
   <si>
-    <t>0500555555</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -710,14 +704,59 @@
     <t>10</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>AddressName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
+    <t>0500500555</t>
+  </si>
+  <si>
+    <t>2-February-1990</t>
+  </si>
+  <si>
+    <t>Clarification Logged -</t>
+  </si>
+  <si>
+    <t>OTP Verified</t>
+  </si>
+  <si>
+    <t>ProfileName</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>PIK</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Assertions added</t>
+  </si>
+  <si>
+    <t>Clarification Logged -Bug - Added Address not displayed, without doing navigation - 
+Script Note : A Work around way of address add functionality tested, location selection not feasible</t>
+  </si>
+  <si>
+    <t>Clarification Logged -A Work around way of address delete functionality tested</t>
+  </si>
+  <si>
+    <t>Products</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -804,7 +843,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,8 +886,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -917,6 +962,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -926,7 +982,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,6 +1057,31 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1616,7 +1697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1632,18 +1713,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1901,7 +1982,7 @@
         <v>162</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>176</v>
@@ -2009,21 +2090,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="92.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="7.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2069,29 +2150,33 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="31">
+      <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
+      <c r="H3" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
@@ -2118,7 +2203,9 @@
       <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
@@ -2145,7 +2232,9 @@
       <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9"/>
@@ -2561,7 +2650,9 @@
       <c r="G22" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9">
@@ -2577,57 +2668,59 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="31">
+    <row r="24" spans="1:9" s="44" customFormat="1" ht="60">
+      <c r="A24" s="39">
         <v>19</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="32"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="31">
+      <c r="G24" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="42" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="44" customFormat="1" ht="30">
+      <c r="A25" s="39">
         <v>20</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="42" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9"/>
@@ -2664,9 +2757,7 @@
       <c r="G27" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="32" t="s">
-        <v>14</v>
-      </c>
+      <c r="H27" s="32"/>
       <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9">
@@ -2801,55 +2892,59 @@
       <c r="H33" s="10"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="31">
+    <row r="34" spans="1:9" s="6" customFormat="1">
+      <c r="A34" s="46">
         <v>26</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="31">
+      <c r="H34" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="47"/>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1">
+      <c r="A35" s="46">
         <v>27</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
+      <c r="H35" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="31">
@@ -3088,28 +3183,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3143,8 +3239,11 @@
       <c r="K1" s="11" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="45" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3155,31 +3254,34 @@
         <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>232</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3187,7 +3289,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>191</v>
@@ -3205,7 +3307,7 @@
         <v>191</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>191</v>
@@ -3213,8 +3315,11 @@
       <c r="K3" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3222,7 +3327,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>191</v>
@@ -3240,13 +3345,16 @@
         <v>191</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>191</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>191</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3260,24 +3368,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="8" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3291,383 +3400,69 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="3">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="3">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="3">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="3">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+        <v>194</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>217</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3677,25 +3472,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3709,68 +3501,50 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>179</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>219</v>
+        <v>179</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3781,22 +3555,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3810,42 +3587,140 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>211</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>217</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>194</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="4">
+        <v>511111112</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3853,22 +3728,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3881,11 +3757,12 @@
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>21</v>
       </c>
@@ -3893,13 +3770,14 @@
         <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>204</v>
+        <v>194</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3909,6 +3787,593 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="3">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="3">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="3">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -3918,10 +4383,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="6" max="8" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3938,16 +4403,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3958,22 +4423,22 @@
         <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3984,22 +4449,22 @@
         <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4010,22 +4475,22 @@
         <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4036,10 +4501,10 @@
         <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>191</v>
@@ -4058,147 +4523,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="4">
-        <v>511111112</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Home Page Test & Address Test Added, Assertions Added & Refactor code inprogress, Edit Profile Test Added
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -12,10 +12,11 @@
     <sheet name="RegistrationAndLogin" sheetId="12" r:id="rId3"/>
     <sheet name="Wishlist" sheetId="14" r:id="rId4"/>
     <sheet name="MyAddresses" sheetId="15" r:id="rId5"/>
-    <sheet name="HomePage" sheetId="18" r:id="rId6"/>
-    <sheet name="ChangePassword" sheetId="16" r:id="rId7"/>
-    <sheet name="CartAndCheckout" sheetId="13" r:id="rId8"/>
-    <sheet name="CustomerPayments" sheetId="17" r:id="rId9"/>
+    <sheet name="CustomerPayments" sheetId="17" r:id="rId6"/>
+    <sheet name="HomePage" sheetId="18" r:id="rId7"/>
+    <sheet name="ChangePassword" sheetId="16" r:id="rId8"/>
+    <sheet name="CartAndCheckout" sheetId="13" r:id="rId9"/>
+    <sheet name="ViewAndEditProfile" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="249">
   <si>
     <t>P_Key</t>
   </si>
@@ -149,9 +150,6 @@
     <t>addNewMadaCard</t>
   </si>
   <si>
-    <t>addNewMasterCard</t>
-  </si>
-  <si>
     <t>checkWalletAmount</t>
   </si>
   <si>
@@ -185,9 +183,6 @@
     <t>As Customer_Payments_Validate that user can Add New "Mada" Card</t>
   </si>
   <si>
-    <t>As Customer_Payments_Validate that user can Add New "Master Card"Card</t>
-  </si>
-  <si>
     <t xml:space="preserve">As Customer_Payments_Validate that user can check wallet amount </t>
   </si>
   <si>
@@ -683,24 +678,12 @@
     <t>Product1</t>
   </si>
   <si>
-    <t>VisaCard</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
     <t>5297412542005689</t>
   </si>
   <si>
-    <t>MadaCard</t>
-  </si>
-  <si>
-    <t>5123456789012346</t>
-  </si>
-  <si>
-    <t>MasterCard</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -722,9 +705,6 @@
     <t>2-February-1990</t>
   </si>
   <si>
-    <t>Clarification Logged -</t>
-  </si>
-  <si>
     <t>OTP Verified</t>
   </si>
   <si>
@@ -738,9 +718,6 @@
   </si>
   <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>Assertions added</t>
   </si>
   <si>
     <t>Clarification Logged -Bug - Added Address not displayed, without doing navigation - 
@@ -751,13 +728,65 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>validateUserProfile</t>
+  </si>
+  <si>
+    <t>As Customer_View Profile_Validate that user can check profile information</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>CardPartialDetails</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>5689</t>
+  </si>
+  <si>
+    <t>View &amp; Edit Profile Tests</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+ -Login to DB Failed 
+    - 1111 OTP is not Working to Register a User 
+    - Getting error when used the same number twice, this will cause the script to fail second time.</t>
+  </si>
+  <si>
+    <t>Clarification Logged - Need a different login data to test change Password, same user is used for other tests which will have conflict</t>
+  </si>
+  <si>
+    <t>Clarification Logged -  Test Step &amp; Verification is generic, Need Clear Verification Step of What to be verified.
+   Just mentioned to check section &amp; those assertion are not quantifiable &amp; clear.</t>
+  </si>
+  <si>
+    <t>Clarification Logged - Seams there is an Application Bug. Adding Mada Card, The Add Card keeps Loading</t>
+  </si>
+  <si>
+    <t>Clarification Logged - Adding Visa Card, displays Payment processing &amp; Payment success was this expected.</t>
+  </si>
+  <si>
+    <t>ViewAndEditProfile</t>
+  </si>
+  <si>
+    <t>automation@gmail.com</t>
+  </si>
+  <si>
+    <t>511111112</t>
+  </si>
+  <si>
+    <t>2000-01-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,6 +869,12 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -982,7 +1017,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,7 +1089,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1082,55 +1116,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="13" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <fill>
         <patternFill>
@@ -1394,22 +1403,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A5:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="WebConfiguration" dataDxfId="39"/>
-    <tableColumn id="2" name="BaseURL" dataDxfId="38"/>
-    <tableColumn id="3" name="Browser" dataDxfId="37"/>
-    <tableColumn id="4" name="Width" dataDxfId="36"/>
-    <tableColumn id="5" name="Height" dataDxfId="35"/>
-    <tableColumn id="6" name="MAXWait" dataDxfId="34"/>
+    <tableColumn id="1" name="WebConfiguration" dataDxfId="33"/>
+    <tableColumn id="2" name="BaseURL" dataDxfId="32"/>
+    <tableColumn id="3" name="Browser" dataDxfId="31"/>
+    <tableColumn id="4" name="Width" dataDxfId="30"/>
+    <tableColumn id="5" name="Height" dataDxfId="29"/>
+    <tableColumn id="6" name="MAXWait" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A13:N19"/>
   <tableColumns count="14">
     <tableColumn id="1" name="MobileConfiguration"/>
@@ -1420,10 +1429,10 @@
     <tableColumn id="6" name="AppName"/>
     <tableColumn id="12" name="AppURL"/>
     <tableColumn id="7" name="AppPackage"/>
-    <tableColumn id="8" name="AppActivity" dataDxfId="32"/>
+    <tableColumn id="8" name="AppActivity" dataDxfId="26"/>
     <tableColumn id="9" name="AppiumURL"/>
     <tableColumn id="10" name="AutomationName"/>
-    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="31"/>
+    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="25"/>
     <tableColumn id="13" name="Project"/>
     <tableColumn id="14" name="Build"/>
   </tableColumns>
@@ -1435,7 +1444,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Platform" dataDxfId="30"/>
+    <tableColumn id="1" name="Platform" dataDxfId="24"/>
     <tableColumn id="2" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1729,10 +1738,10 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -1743,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1754,27 +1763,27 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
         <v>126</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>127</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>128</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>129</v>
-      </c>
-      <c r="E5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1782,27 +1791,27 @@
         <v>4</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="E6" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>135</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D7" s="19">
         <v>1920</v>
@@ -1817,11 +1826,11 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D8" s="19">
         <v>1920</v>
@@ -1836,11 +1845,11 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D9" s="20">
         <v>1080</v>
@@ -1855,7 +1864,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1866,7 +1875,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -1877,46 +1886,46 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
         <v>143</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>144</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>145</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="H13" t="s">
         <v>148</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>149</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="L13" t="s">
         <v>152</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>153</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>154</v>
-      </c>
-      <c r="M13" t="s">
-        <v>155</v>
-      </c>
-      <c r="N13" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1924,146 +1933,146 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" t="s">
         <v>157</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>158</v>
-      </c>
-      <c r="D14" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D15" s="30">
         <v>11</v>
       </c>
       <c r="E15" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" t="s">
         <v>163</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>164</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="L15" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="K15" t="s">
-        <v>168</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" t="s">
         <v>164</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>166</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="L16" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="K16" t="s">
-        <v>168</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="B17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="E17" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" t="s">
         <v>162</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="G17" t="s">
         <v>175</v>
       </c>
-      <c r="E17" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" t="s">
         <v>164</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J17" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="K17" t="s">
+        <v>166</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="M17" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="H17" t="s">
-        <v>165</v>
-      </c>
-      <c r="I17" t="s">
-        <v>166</v>
-      </c>
-      <c r="J17" s="28" t="s">
+      <c r="N17" s="24" t="s">
         <v>178</v>
-      </c>
-      <c r="K17" t="s">
-        <v>168</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E19" s="23"/>
     </row>
@@ -2086,12 +2095,106 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2149,33 +2252,33 @@
       <c r="H2" s="10"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="39">
+    <row r="3" spans="1:9" ht="75">
+      <c r="A3" s="53">
         <v>1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>231</v>
+      <c r="H3" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2197,15 +2300,13 @@
       <c r="F4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>237</v>
-      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
@@ -2226,15 +2327,13 @@
       <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>237</v>
-      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9"/>
@@ -2260,19 +2359,19 @@
         <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -2287,13 +2386,13 @@
         <v>32</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>12</v>
@@ -2312,19 +2411,19 @@
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -2339,19 +2438,19 @@
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -2366,13 +2465,13 @@
         <v>32</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>12</v>
@@ -2391,19 +2490,19 @@
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -2418,19 +2517,19 @@
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -2445,19 +2544,19 @@
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -2466,19 +2565,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>12</v>
@@ -2491,19 +2590,19 @@
         <v>13</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G16" s="31" t="s">
         <v>12</v>
@@ -2516,19 +2615,19 @@
         <v>14</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G17" s="31" t="s">
         <v>12</v>
@@ -2541,25 +2640,25 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -2568,19 +2667,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" s="31" t="s">
         <v>12</v>
@@ -2606,21 +2705,21 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -2633,21 +2732,21 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -2658,7 +2757,7 @@
     <row r="23" spans="1:9">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2668,64 +2767,68 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" s="44" customFormat="1" ht="60">
-      <c r="A24" s="39">
+    <row r="24" spans="1:9" s="43" customFormat="1" ht="60">
+      <c r="A24" s="38">
         <v>19</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="43" customFormat="1" ht="30">
+      <c r="A25" s="38">
+        <v>20</v>
+      </c>
+      <c r="B25" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="40" t="s">
+      <c r="C25" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="39" t="s">
+      <c r="F25" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="42" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="44" customFormat="1" ht="30">
-      <c r="A25" s="39">
-        <v>20</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="42" t="s">
-        <v>239</v>
+      <c r="H25" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="I25" s="41" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2735,30 +2838,32 @@
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="45">
       <c r="A27" s="31">
         <v>21</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="33" t="s">
         <v>75</v>
       </c>
+      <c r="C27" s="54" t="s">
+        <v>73</v>
+      </c>
       <c r="D27" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="36" t="s">
-        <v>76</v>
+      <c r="F27" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="G27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="I27" s="41" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9"/>
@@ -2773,7 +2878,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="30">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -2781,26 +2886,28 @@
         <v>38</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="I29" s="41" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -2808,368 +2915,281 @@
         <v>39</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="38" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="1">
+      <c r="I30" s="41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1">
+      <c r="A31" s="45">
         <v>24</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="C31" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="31" t="s">
+      <c r="F31" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="2"/>
+      <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="31">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" s="6" customFormat="1">
+      <c r="A33" s="45">
         <v>25</v>
       </c>
-      <c r="B32" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="32" t="s">
+      <c r="B33" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="46"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1">
+      <c r="A35" s="45">
+        <v>26</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E35" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="31" t="s">
+      <c r="F35" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" s="6" customFormat="1">
-      <c r="A34" s="46">
-        <v>26</v>
-      </c>
-      <c r="B34" s="47" t="s">
+      <c r="H35" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="46"/>
+    </row>
+    <row r="36" spans="1:9" s="6" customFormat="1">
+      <c r="A36" s="45">
+        <v>27</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="46"/>
+    </row>
+    <row r="37" spans="1:9" ht="60">
+      <c r="A37" s="31">
+        <v>28</v>
+      </c>
+      <c r="B37" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="47"/>
-    </row>
-    <row r="35" spans="1:9" s="6" customFormat="1">
-      <c r="A35" s="46">
-        <v>27</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="47" t="s">
+      <c r="C37" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="32" t="s">
         <v>82</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="47"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="31">
-        <v>28</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="31">
-        <v>29</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>85</v>
       </c>
       <c r="E37" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="I37" s="41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60">
       <c r="A38" s="31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>79</v>
+        <v>94</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G38" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="I38" s="41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60">
       <c r="A39" s="31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>79</v>
+        <v>95</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E39" s="32" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G39" s="31" t="s">
         <v>12</v>
       </c>
       <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60">
+      <c r="A40" s="31">
+        <v>31</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="32"/>
+      <c r="I40" s="41" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G11 G23:G25 G40:G1048576 G1:G7 G28:G32">
-    <cfRule type="cellIs" dxfId="29" priority="53" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="23" priority="53" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="54" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20 G22:G25">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G25">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G27">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34:G39">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G18">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G10">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"NO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H40">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
@@ -3186,7 +3206,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L1" sqref="L1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3213,34 +3233,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>233</v>
+        <v>188</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3251,34 +3271,34 @@
         <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="43" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>235</v>
+        <v>225</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3289,34 +3309,34 @@
         <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="L3" s="38" t="s">
-        <v>234</v>
+        <v>189</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3327,34 +3347,34 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="L4" s="38" t="s">
-        <v>234</v>
+        <v>189</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3371,7 +3391,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3394,22 +3414,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3417,25 +3437,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3443,25 +3463,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3472,10 +3492,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3485,6 +3505,7 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3495,16 +3516,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3512,19 +3533,19 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>228</v>
+        <v>177</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3532,19 +3553,19 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>228</v>
+        <v>177</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3554,6 +3575,159 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -3581,22 +3755,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3604,25 +3778,25 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3630,25 +3804,25 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3656,16 +3830,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3673,16 +3847,16 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="4">
         <v>511111112</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3690,16 +3864,16 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3707,16 +3881,16 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3726,12 +3900,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3740,11 +3914,10 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3752,32 +3925,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
+      </c>
+      <c r="E2" s="4">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -3786,12 +3957,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3804,14 +3975,15 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3819,40 +3991,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="3">
         <v>4</v>
       </c>
@@ -3860,40 +4035,43 @@
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>191</v>
+      <c r="I2" s="4">
+        <v>2</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>5</v>
       </c>
@@ -3901,10 +4079,10 @@
         <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3915,8 +4093,9 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="3">
         <v>6</v>
       </c>
@@ -3924,40 +4103,41 @@
         <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4005550000000000</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>7</v>
       </c>
@@ -3965,40 +4145,41 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>207</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -4006,40 +4187,41 @@
         <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3">
         <v>9</v>
       </c>
@@ -4047,40 +4229,41 @@
         <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>207</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3">
         <v>10</v>
       </c>
@@ -4088,40 +4271,41 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>208</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
         <v>11</v>
       </c>
@@ -4129,394 +4313,248 @@
         <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>209</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>210</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="3">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3">
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>210</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>189</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="3">
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Password Test Added.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="252">
   <si>
     <t>P_Key</t>
   </si>
@@ -780,12 +780,22 @@
   </si>
   <si>
     <t>2000-01-01</t>
+  </si>
+  <si>
+    <t>OldPassword</t>
+  </si>
+  <si>
+    <t>Password changed successfully</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -1017,7 +1027,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1089,7 +1099,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1098,9 +1107,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1130,170 +1136,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1403,22 +1256,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A5:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="WebConfiguration" dataDxfId="33"/>
-    <tableColumn id="2" name="BaseURL" dataDxfId="32"/>
-    <tableColumn id="3" name="Browser" dataDxfId="31"/>
-    <tableColumn id="4" name="Width" dataDxfId="30"/>
-    <tableColumn id="5" name="Height" dataDxfId="29"/>
-    <tableColumn id="6" name="MAXWait" dataDxfId="28"/>
+    <tableColumn id="1" name="WebConfiguration" dataDxfId="11"/>
+    <tableColumn id="2" name="BaseURL" dataDxfId="10"/>
+    <tableColumn id="3" name="Browser" dataDxfId="9"/>
+    <tableColumn id="4" name="Width" dataDxfId="8"/>
+    <tableColumn id="5" name="Height" dataDxfId="7"/>
+    <tableColumn id="6" name="MAXWait" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A13:N19"/>
   <tableColumns count="14">
     <tableColumn id="1" name="MobileConfiguration"/>
@@ -1429,10 +1282,10 @@
     <tableColumn id="6" name="AppName"/>
     <tableColumn id="12" name="AppURL"/>
     <tableColumn id="7" name="AppPackage"/>
-    <tableColumn id="8" name="AppActivity" dataDxfId="26"/>
+    <tableColumn id="8" name="AppActivity" dataDxfId="4"/>
     <tableColumn id="9" name="AppiumURL"/>
     <tableColumn id="10" name="AutomationName"/>
-    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="25"/>
+    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="3"/>
     <tableColumn id="13" name="Project"/>
     <tableColumn id="14" name="Build"/>
   </tableColumns>
@@ -1444,7 +1297,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Platform" dataDxfId="24"/>
+    <tableColumn id="1" name="Platform" dataDxfId="2"/>
     <tableColumn id="2" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1706,7 +1559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1722,18 +1575,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2105,16 +1958,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.7109375" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2130,7 +1983,7 @@
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="42" t="s">
         <v>226</v>
       </c>
       <c r="F1" s="11" t="s">
@@ -2162,7 +2015,7 @@
       <c r="D2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>227</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -2171,13 +2024,13 @@
       <c r="G2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="40" t="s">
         <v>247</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="40" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2193,21 +2046,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="92.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="7.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="55.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2253,31 +2106,31 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="75">
-      <c r="A3" s="53">
+      <c r="A3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="39" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2300,7 +2153,7 @@
       <c r="F4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -2327,7 +2180,7 @@
       <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -2367,7 +2220,7 @@
       <c r="F7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -2419,7 +2272,7 @@
       <c r="F9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -2446,7 +2299,7 @@
       <c r="F10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -2498,7 +2351,7 @@
       <c r="F12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -2525,7 +2378,7 @@
       <c r="F13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -2552,7 +2405,7 @@
       <c r="F14" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -2654,7 +2507,7 @@
       <c r="F18" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -2719,7 +2572,7 @@
       <c r="F21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -2746,7 +2599,7 @@
       <c r="F22" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -2767,61 +2620,61 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" s="43" customFormat="1" ht="60">
-      <c r="A24" s="38">
+    <row r="24" spans="1:9" s="41" customFormat="1" ht="60">
+      <c r="A24" s="37">
         <v>19</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="39" t="s">
+      <c r="H24" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="39" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="43" customFormat="1" ht="30">
-      <c r="A25" s="38">
+    <row r="25" spans="1:9" s="41" customFormat="1" ht="30">
+      <c r="A25" s="37">
         <v>20</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="39" t="s">
+      <c r="H25" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="39" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2839,29 +2692,31 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="45">
-      <c r="A27" s="31">
+      <c r="A27" s="43">
         <v>21</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="41" t="s">
+      <c r="G27" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="I27" s="39" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2897,13 +2752,13 @@
       <c r="F29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G29" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="41" t="s">
+      <c r="I29" s="39" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2926,42 +2781,42 @@
       <c r="F30" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="38" t="s">
+      <c r="G30" s="37" t="s">
         <v>12</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="41" t="s">
+      <c r="I30" s="39" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1">
-      <c r="A31" s="45">
+      <c r="A31" s="43">
         <v>24</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="38" t="s">
+      <c r="G31" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="46" t="s">
+      <c r="H31" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="46"/>
+      <c r="I31" s="44"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="9"/>
@@ -2977,7 +2832,7 @@
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" s="6" customFormat="1">
-      <c r="A33" s="45">
+      <c r="A33" s="43">
         <v>25</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -2986,22 +2841,22 @@
       <c r="C33" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="44" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="46" t="s">
+      <c r="H33" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="46"/>
+      <c r="I33" s="44"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="9"/>
@@ -3017,58 +2872,58 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" s="6" customFormat="1">
-      <c r="A35" s="45">
+      <c r="A35" s="43">
         <v>26</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="46" t="s">
+      <c r="F35" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="38" t="s">
+      <c r="G35" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="46" t="s">
+      <c r="H35" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="46"/>
+      <c r="I35" s="44"/>
     </row>
     <row r="36" spans="1:9" s="6" customFormat="1">
-      <c r="A36" s="45">
+      <c r="A36" s="43">
         <v>27</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="F36" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="38" t="s">
+      <c r="G36" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="46" t="s">
+      <c r="H36" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I36" s="46"/>
+      <c r="I36" s="44"/>
     </row>
     <row r="37" spans="1:9" ht="60">
       <c r="A37" s="31">
@@ -3077,7 +2932,7 @@
       <c r="B37" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="32" t="s">
@@ -3093,7 +2948,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="32"/>
-      <c r="I37" s="41" t="s">
+      <c r="I37" s="39" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3104,7 +2959,7 @@
       <c r="B38" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="35" t="s">
         <v>77</v>
       </c>
       <c r="D38" s="32" t="s">
@@ -3120,7 +2975,7 @@
         <v>12</v>
       </c>
       <c r="H38" s="32"/>
-      <c r="I38" s="41" t="s">
+      <c r="I38" s="39" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3131,7 +2986,7 @@
       <c r="B39" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>77</v>
       </c>
       <c r="D39" s="32" t="s">
@@ -3147,7 +3002,7 @@
         <v>12</v>
       </c>
       <c r="H39" s="32"/>
-      <c r="I39" s="41" t="s">
+      <c r="I39" s="39" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3158,7 +3013,7 @@
       <c r="B40" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="35" t="s">
         <v>77</v>
       </c>
       <c r="D40" s="32" t="s">
@@ -3174,17 +3029,17 @@
         <v>12</v>
       </c>
       <c r="H40" s="32"/>
-      <c r="I40" s="41" t="s">
+      <c r="I40" s="39" t="s">
         <v>242</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="23" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3206,23 +3061,23 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L3"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3259,7 +3114,7 @@
       <c r="K1" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="42" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3279,13 +3134,13 @@
       <c r="E2" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="40" t="s">
         <v>223</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="40" t="s">
         <v>224</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -3297,7 +3152,7 @@
       <c r="K2" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3335,7 +3190,7 @@
       <c r="K3" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="36" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3373,7 +3228,7 @@
       <c r="K4" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3396,14 +3251,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3492,7 +3347,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -3500,12 +3355,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3544,7 +3399,7 @@
       <c r="E2" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3564,7 +3419,7 @@
       <c r="E3" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="36" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3584,16 +3439,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3624,7 +3479,7 @@
       <c r="I1" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="42" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3656,7 +3511,7 @@
       <c r="I2" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="46" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3688,7 +3543,7 @@
       <c r="I3" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="J3" s="47" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3737,14 +3592,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3902,22 +3757,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="28.85546875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3931,10 +3789,19 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
         <v>21</v>
       </c>
@@ -3949,6 +3816,15 @@
       </c>
       <c r="E2" s="4">
         <v>123456</v>
+      </c>
+      <c r="F2" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G2">
+        <v>123456</v>
+      </c>
+      <c r="H2" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3961,26 +3837,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>

<commit_message>
Cart Test Failure Fixing & Adding Assertions
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -795,7 +795,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -1559,7 +1558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1575,18 +1574,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1958,16 +1957,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.7109375" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2046,21 +2045,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="92.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="7.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="55.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2221,7 +2220,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>229</v>
@@ -2711,7 +2710,7 @@
         <v>74</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>251</v>
+        <v>12</v>
       </c>
       <c r="H27" s="44" t="s">
         <v>229</v>
@@ -3066,18 +3065,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3251,14 +3250,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3347,7 +3346,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -3355,12 +3354,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3439,16 +3438,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3592,14 +3591,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3765,14 +3764,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="28.85546875" collapsed="false"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3837,26 +3836,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">

</xml_diff>

<commit_message>
Cart Test Added & Fixed one Test
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="8"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
     <sheet name="Controller" sheetId="1" r:id="rId2"/>
-    <sheet name="RegistrationAndLogin" sheetId="12" r:id="rId3"/>
-    <sheet name="Wishlist" sheetId="14" r:id="rId4"/>
-    <sheet name="MyAddresses" sheetId="15" r:id="rId5"/>
-    <sheet name="CustomerPayments" sheetId="17" r:id="rId6"/>
-    <sheet name="HomePage" sheetId="18" r:id="rId7"/>
-    <sheet name="ChangePassword" sheetId="16" r:id="rId8"/>
-    <sheet name="CartAndCheckout" sheetId="13" r:id="rId9"/>
+    <sheet name="CartAndCheckout" sheetId="13" r:id="rId3"/>
+    <sheet name="RegistrationAndLogin" sheetId="12" r:id="rId4"/>
+    <sheet name="Wishlist" sheetId="14" r:id="rId5"/>
+    <sheet name="MyAddresses" sheetId="15" r:id="rId6"/>
+    <sheet name="CustomerPayments" sheetId="17" r:id="rId7"/>
+    <sheet name="HomePage" sheetId="18" r:id="rId8"/>
+    <sheet name="ChangePassword" sheetId="16" r:id="rId9"/>
     <sheet name="ViewAndEditProfile" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="255">
   <si>
     <t>P_Key</t>
   </si>
@@ -634,9 +634,6 @@
   </si>
   <si>
     <t>4005550000000001</t>
-  </si>
-  <si>
-    <t>automationteam</t>
   </si>
   <si>
     <t>350</t>
@@ -789,6 +786,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>DeliveryType</t>
+  </si>
+  <si>
+    <t>Self Pickup</t>
+  </si>
+  <si>
+    <t>Cash On Delivery</t>
+  </si>
+  <si>
+    <t>automation</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1035,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1139,6 +1148,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1843,7 +1855,7 @@
         <v>160</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>174</v>
@@ -1961,12 +1973,12 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1983,7 +1995,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>13</v>
@@ -2006,7 +2018,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>193</v>
@@ -2015,22 +2027,22 @@
         <v>192</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="40" t="s">
         <v>246</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>247</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2045,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2127,10 +2139,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2220,37 +2232,39 @@
         <v>52</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>251</v>
+        <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>229</v>
+        <v>14</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="31">
+      <c r="A8" s="43">
         <v>5</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
+      <c r="G8" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="44"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
@@ -2275,7 +2289,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -2302,7 +2316,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -2354,7 +2368,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -2381,7 +2395,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -2408,7 +2422,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -2510,7 +2524,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -2642,10 +2656,10 @@
         <v>12</v>
       </c>
       <c r="H24" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="I24" s="39" t="s">
         <v>229</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="41" customFormat="1" ht="30">
@@ -2671,10 +2685,10 @@
         <v>12</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I25" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2713,10 +2727,10 @@
         <v>12</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I27" s="39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2758,7 +2772,7 @@
         <v>14</v>
       </c>
       <c r="I29" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30">
@@ -2787,7 +2801,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1">
@@ -2820,7 +2834,7 @@
     <row r="32" spans="1:9">
       <c r="A32" s="9"/>
       <c r="B32" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2835,10 +2849,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>76</v>
@@ -2847,7 +2861,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G33" s="43" t="s">
         <v>12</v>
@@ -2948,7 +2962,7 @@
       </c>
       <c r="H37" s="32"/>
       <c r="I37" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60">
@@ -2975,7 +2989,7 @@
       </c>
       <c r="H38" s="32"/>
       <c r="I38" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="60">
@@ -3002,7 +3016,7 @@
       </c>
       <c r="H39" s="32"/>
       <c r="I39" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="60">
@@ -3029,7 +3043,7 @@
       </c>
       <c r="H40" s="32"/>
       <c r="I40" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3057,10 +3071,674 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="3">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="3">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="3">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="3">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="3">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="3">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="3">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="3">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="3">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="3">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3114,7 +3792,7 @@
         <v>188</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3128,19 +3806,19 @@
         <v>189</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>190</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>192</v>
@@ -3149,10 +3827,10 @@
         <v>192</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3190,7 +3868,7 @@
         <v>189</v>
       </c>
       <c r="L3" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3228,7 +3906,7 @@
         <v>189</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3240,7 +3918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -3274,16 +3952,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3300,16 +3978,16 @@
         <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3326,16 +4004,16 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3344,7 +4022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -3376,10 +4054,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3399,7 +4077,7 @@
         <v>177</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3419,7 +4097,7 @@
         <v>177</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3428,12 +4106,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3479,7 +4157,7 @@
         <v>199</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3499,19 +4177,19 @@
         <v>201</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3528,22 +4206,22 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="J3" s="47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3581,7 +4259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -3615,16 +4293,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3641,16 +4319,16 @@
         <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3667,16 +4345,16 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3754,7 +4432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3768,10 +4446,10 @@
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3788,10 +4466,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>187</v>
@@ -3823,613 +4501,7 @@
         <v>123456</v>
       </c>
       <c r="H2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="3">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I2" s="4">
-        <v>2</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="3">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="3">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K4" s="4">
-        <v>4005550000000000</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="3">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="3">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="3">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="3">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="3">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="3">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="3">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="3">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>189</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporary commit if code flow
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="262">
   <si>
     <t>P_Key</t>
   </si>
@@ -642,13 +642,7 @@
     <t>0525</t>
   </si>
   <si>
-    <t>CASHONDELIVERY</t>
-  </si>
-  <si>
     <t>MADA</t>
-  </si>
-  <si>
-    <t>MASTERCARD</t>
   </si>
   <si>
     <t>VISA</t>
@@ -798,6 +792,33 @@
   </si>
   <si>
     <t>automation</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Apple Pay</t>
+  </si>
+  <si>
+    <t>5123456789012346</t>
+  </si>
+  <si>
+    <t>2346</t>
+  </si>
+  <si>
+    <t>MASTER</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>12 Pro</t>
+  </si>
+  <si>
+    <t>0511111114</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1591,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1581,7 +1602,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
@@ -1855,7 +1876,7 @@
         <v>160</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>174</v>
@@ -1938,7 +1959,42 @@
       <c r="A19" t="s">
         <v>181</v>
       </c>
-      <c r="E19" s="23"/>
+      <c r="B19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" t="s">
+        <v>164</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1948,13 +2004,14 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J17" r:id="rId1"/>
+    <hyperlink ref="J19" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="3">
-    <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1995,7 +2052,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>13</v>
@@ -2018,7 +2075,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>193</v>
@@ -2027,22 +2084,22 @@
         <v>192</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2057,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2139,10 +2196,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2232,7 +2289,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>12</v>
+        <v>248</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>14</v>
@@ -2259,7 +2316,7 @@
         <v>53</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="H8" s="44" t="s">
         <v>14</v>
@@ -2289,7 +2346,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -2316,7 +2373,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -2368,7 +2425,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -2395,7 +2452,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -2422,7 +2479,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -2524,7 +2581,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -2656,10 +2713,10 @@
         <v>12</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I24" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="41" customFormat="1" ht="30">
@@ -2685,10 +2742,10 @@
         <v>12</v>
       </c>
       <c r="H25" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="I25" s="39" t="s">
         <v>228</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2727,10 +2784,10 @@
         <v>12</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I27" s="39" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2772,7 +2829,7 @@
         <v>14</v>
       </c>
       <c r="I29" s="39" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30">
@@ -2801,7 +2858,7 @@
         <v>14</v>
       </c>
       <c r="I30" s="39" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1">
@@ -2834,7 +2891,7 @@
     <row r="32" spans="1:9">
       <c r="A32" s="9"/>
       <c r="B32" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2849,10 +2906,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>76</v>
@@ -2861,7 +2918,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G33" s="43" t="s">
         <v>12</v>
@@ -2962,7 +3019,7 @@
       </c>
       <c r="H37" s="32"/>
       <c r="I37" s="39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60">
@@ -2989,7 +3046,7 @@
       </c>
       <c r="H38" s="32"/>
       <c r="I38" s="39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="60">
@@ -3016,7 +3073,7 @@
       </c>
       <c r="H39" s="32"/>
       <c r="I39" s="39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="60">
@@ -3043,7 +3100,7 @@
       </c>
       <c r="H40" s="32"/>
       <c r="I40" s="39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3073,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3111,25 +3168,25 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>195</v>
@@ -3161,36 +3218,40 @@
         <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>214</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L2" s="4" t="s">
         <v>189</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>254</v>
+        <v>189</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3207,28 +3268,28 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>214</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>189</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>189</v>
@@ -3257,31 +3318,37 @@
         <v>192</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>234</v>
+      </c>
       <c r="L4" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>201</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>203</v>
@@ -3301,22 +3368,28 @@
         <v>192</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L5" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>189</v>
@@ -3345,22 +3418,28 @@
         <v>192</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L6" s="4" t="s">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>189</v>
@@ -3389,34 +3468,40 @@
         <v>192</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="P7" s="4" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3433,34 +3518,40 @@
         <v>192</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K8" s="47" t="s">
+        <v>235</v>
+      </c>
       <c r="L8" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -3477,34 +3568,40 @@
         <v>192</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K9" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="P9" s="4" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -3521,22 +3618,28 @@
         <v>192</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L10" s="4" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>189</v>
@@ -3565,20 +3668,26 @@
         <v>192</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L11" s="4" t="s">
         <v>189</v>
       </c>
@@ -3609,20 +3718,26 @@
         <v>192</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L12" s="4" t="s">
         <v>189</v>
       </c>
@@ -3653,22 +3768,28 @@
         <v>192</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L13" s="4" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>189</v>
@@ -3697,20 +3818,26 @@
         <v>192</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>189</v>
       </c>
@@ -3792,7 +3919,7 @@
         <v>188</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3806,19 +3933,19 @@
         <v>189</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>190</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>191</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>192</v>
@@ -3827,10 +3954,10 @@
         <v>192</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3868,7 +3995,7 @@
         <v>189</v>
       </c>
       <c r="L3" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3906,7 +4033,7 @@
         <v>189</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3952,16 +4079,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3978,16 +4105,16 @@
         <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4004,16 +4131,16 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4054,10 +4181,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4077,7 +4204,7 @@
         <v>177</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4097,7 +4224,7 @@
         <v>177</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -4111,7 +4238,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4157,7 +4284,7 @@
         <v>199</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4177,19 +4304,19 @@
         <v>201</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>203</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4206,13 +4333,13 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>202</v>
@@ -4221,7 +4348,7 @@
         <v>203</v>
       </c>
       <c r="J3" s="47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4293,16 +4420,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>194</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4319,16 +4446,16 @@
         <v>192</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4345,16 +4472,16 @@
         <v>192</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4436,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4466,10 +4593,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G1" s="42" t="s">
         <v>187</v>
@@ -4485,23 +4612,23 @@
       <c r="B2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>193</v>
+      <c r="C2" s="40" t="s">
+        <v>261</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="4">
-        <v>123456</v>
+      <c r="E2" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="F2" s="4">
-        <v>123456</v>
+        <v>123457</v>
       </c>
       <c r="G2">
-        <v>123456</v>
+        <v>123457</v>
       </c>
       <c r="H2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Failures Fixed & Status Updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="8"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="268">
   <si>
     <t>P_Key</t>
   </si>
@@ -72,9 +72,6 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>Registration&amp;Login Tests</t>
   </si>
   <si>
@@ -708,16 +705,6 @@
     <t>PIK</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Clarification Logged -Bug - Added Address not displayed, without doing navigation - 
-Script Note : A Work around way of address add functionality tested, location selection not feasible</t>
-  </si>
-  <si>
-    <t>Clarification Logged -A Work around way of address delete functionality tested</t>
-  </si>
-  <si>
     <t>Products</t>
   </si>
   <si>
@@ -740,27 +727,12 @@
   </si>
   <si>
     <t>View &amp; Edit Profile Tests</t>
-  </si>
-  <si>
-    <t>Clarification Logged
- -Login to DB Failed 
-    - 1111 OTP is not Working to Register a User 
-    - Getting error when used the same number twice, this will cause the script to fail second time.</t>
-  </si>
-  <si>
-    <t>Clarification Logged - Need a different login data to test change Password, same user is used for other tests which will have conflict</t>
   </si>
   <si>
     <t>Clarification Logged -  Test Step &amp; Verification is generic, Need Clear Verification Step of What to be verified.
    Just mentioned to check section &amp; those assertion are not quantifiable &amp; clear.</t>
   </si>
   <si>
-    <t>Clarification Logged - Seams there is an Application Bug. Adding Mada Card, The Add Card keeps Loading</t>
-  </si>
-  <si>
-    <t>Clarification Logged - Adding Visa Card, displays Payment processing &amp; Payment success was this expected.</t>
-  </si>
-  <si>
     <t>ViewAndEditProfile</t>
   </si>
   <si>
@@ -779,9 +751,6 @@
     <t>Password changed successfully</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>DeliveryType</t>
   </si>
   <si>
@@ -819,6 +788,61 @@
   </si>
   <si>
     <t>0511111114</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarification Logged
+    - Which collection to refer for OTP No clear step to get OTP from DB &amp; Use for Registration
+    - Getting error when used the same number twice, this will cause the script to fail second time. </t>
+  </si>
+  <si>
+    <t>Clarification Logged
+    - App Issue, Add to cart not Working</t>
+  </si>
+  <si>
+    <t>addNewMasterCard</t>
+  </si>
+  <si>
+    <t>TC-032</t>
+  </si>
+  <si>
+    <t>As Customer_Payments_Validate that user can Add New "Master" Card</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Piktestuser</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+  - Bug - Added Address not displayed, without doing navigation
+Script Note : A Work around way of address add functionality tested and location selection not feasible.</t>
+  </si>
+  <si>
+    <t>Completed 
+- Note Change TestData else reset credential for every Run</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+- Bug in Add Address 
+- A Work around way of add address done to test delete functionality</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+- Adding Visa Card, displays Payment processing &amp; Payment success was this expected.</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+- Seams there is an Application Bug. Adding Mada Card, The Add Card keeps Loading</t>
+  </si>
+  <si>
+    <t>Automa</t>
   </si>
 </sst>
 </file>
@@ -917,7 +941,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +987,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,7 +1086,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1091,10 +1121,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1150,14 +1176,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="13" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1166,11 +1187,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1602,7 +1639,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
@@ -1623,194 +1660,194 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
         <v>119</v>
-      </c>
-      <c r="B1" t="s">
-        <v>120</v>
       </c>
       <c r="F1">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>125</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>126</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>127</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>128</v>
       </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="17">
+        <v>1920</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1080</v>
+      </c>
+      <c r="F7" s="17">
+        <v>5</v>
+      </c>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="19">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="17">
         <v>1920</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E8" s="18">
         <v>1080</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F8" s="17">
         <v>5</v>
       </c>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19" t="s">
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="19">
-        <v>1920</v>
-      </c>
-      <c r="E8" s="20">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="18">
         <v>1080</v>
       </c>
-      <c r="F8" s="19">
+      <c r="E9" s="18">
+        <v>1080</v>
+      </c>
+      <c r="F9" s="17">
         <v>5</v>
       </c>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20" t="s">
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="20">
-        <v>1080</v>
-      </c>
-      <c r="E9" s="20">
-        <v>1080</v>
-      </c>
-      <c r="F9" s="19">
-        <v>5</v>
-      </c>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="19" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" t="s">
         <v>141</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>142</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>143</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>144</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" t="s">
         <v>146</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>147</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>148</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="K13" t="s">
         <v>150</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>151</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>152</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>153</v>
-      </c>
-      <c r="N13" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1818,182 +1855,182 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" t="s">
         <v>155</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>156</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>157</v>
-      </c>
-      <c r="E14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="D15" s="28">
+        <v>11</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D15" s="30">
-        <v>11</v>
-      </c>
-      <c r="E15" s="23" t="s">
+      <c r="F15" t="s">
         <v>161</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="K15" t="s">
         <v>165</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" s="23" t="s">
         <v>166</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
         <v>168</v>
       </c>
-      <c r="B16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>174</v>
+      <c r="C16" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="F16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" t="s">
         <v>162</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>163</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="K16" t="s">
         <v>165</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" s="23" t="s">
         <v>166</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
         <v>171</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>170</v>
+      <c r="E17" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="F17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" t="s">
         <v>162</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
+        <v>163</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="H17" t="s">
-        <v>163</v>
-      </c>
-      <c r="I17" t="s">
-        <v>164</v>
-      </c>
-      <c r="J17" s="28" t="s">
+      <c r="K17" t="s">
+        <v>165</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="K17" t="s">
-        <v>166</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="M17" s="24" t="s">
+      <c r="N17" s="22" t="s">
         <v>177</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>179</v>
-      </c>
-      <c r="B18" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>260</v>
+        <v>171</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>251</v>
       </c>
       <c r="F19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" t="s">
         <v>162</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
+        <v>163</v>
+      </c>
+      <c r="J19" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="H19" t="s">
-        <v>163</v>
-      </c>
-      <c r="I19" t="s">
-        <v>164</v>
-      </c>
-      <c r="J19" s="28" t="s">
+      <c r="L19" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="L19" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="M19" s="24" t="s">
+      <c r="N19" s="22" t="s">
         <v>177</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2046,28 +2083,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>223</v>
+      <c r="E1" s="40" t="s">
+        <v>222</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2075,31 +2112,31 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>224</v>
+        <v>191</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>223</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>244</v>
+        <v>235</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>236</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>245</v>
+        <v>190</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2112,20 +2149,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="92" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="7.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
@@ -2163,7 +2200,7 @@
     <row r="2" spans="1:9" s="6" customFormat="1">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2174,92 +2211,94 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="75">
-      <c r="A3" s="51">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="48">
+        <v>2</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="38" t="s">
+      <c r="C4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E4" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="H4" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="48">
+        <v>3</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2"/>
+      <c r="H5" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2269,351 +2308,361 @@
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="41">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="43">
-        <v>5</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="44"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="2"/>
+      <c r="I8" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="H9" s="2"/>
+      <c r="I9" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="29">
+        <v>8</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="31">
-        <v>8</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="H11" s="30"/>
+      <c r="I11" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="H12" s="2"/>
+      <c r="I12" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="H13" s="2"/>
+      <c r="I13" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="29">
+        <v>12</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G15" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="31">
+      <c r="H15" s="30"/>
+      <c r="I15" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30">
+      <c r="A16" s="29">
+        <v>13</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="32" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30">
+      <c r="A17" s="29">
+        <v>14</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="31" t="s">
+      <c r="F17" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="31">
-        <v>13</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="31">
-        <v>14</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="H17" s="30"/>
+      <c r="I17" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30">
+      <c r="A19" s="29">
+        <v>16</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G19" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="31">
-        <v>16</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="37" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="9"/>
       <c r="B20" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2624,63 +2673,67 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="1">
+      <c r="A21" s="48">
         <v>17</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="48">
+        <v>18</v>
+      </c>
+      <c r="B22" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C22" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F22" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G22" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="2"/>
+      <c r="H22" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I22" s="49" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2690,68 +2743,68 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" s="41" customFormat="1" ht="60">
-      <c r="A24" s="37">
+    <row r="24" spans="1:9" s="39" customFormat="1" ht="75">
+      <c r="A24" s="48">
         <v>19</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="39" customFormat="1" ht="60">
+      <c r="A25" s="48">
+        <v>20</v>
+      </c>
+      <c r="B25" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="38" t="s">
+      <c r="C25" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E25" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="50" t="s">
+      <c r="F25" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G25" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="41" customFormat="1" ht="30">
-      <c r="A25" s="37">
-        <v>20</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>228</v>
+      <c r="H25" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2761,39 +2814,39 @@
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" ht="45">
-      <c r="A27" s="43">
+    <row r="27" spans="1:9" ht="30">
+      <c r="A27" s="48">
         <v>21</v>
       </c>
-      <c r="B27" s="44" t="s">
-        <v>75</v>
+      <c r="B27" s="49" t="s">
+        <v>74</v>
       </c>
       <c r="C27" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>238</v>
+      <c r="H27" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I27" s="51" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9"/>
       <c r="B28" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2803,304 +2856,341 @@
       <c r="H28" s="10"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" ht="30">
-      <c r="A29" s="1">
+    <row r="29" spans="1:9" ht="45">
+      <c r="A29" s="48">
         <v>22</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I29" s="37" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45">
+      <c r="A30" s="48">
+        <v>23</v>
+      </c>
+      <c r="B30" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F30" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G30" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="30">
-      <c r="A30" s="1">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2" t="s">
+      <c r="H30" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I30" s="37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" ht="30">
+      <c r="A31" s="48">
+        <v>24</v>
+      </c>
+      <c r="B31" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C31" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F31" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G31" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="39" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="6" customFormat="1">
-      <c r="A31" s="43">
-        <v>24</v>
-      </c>
-      <c r="B31" s="44" t="s">
+      <c r="H31" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I31" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="6" customFormat="1" ht="45">
+      <c r="A32" s="48">
+        <v>32</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>256</v>
+      </c>
+      <c r="C32" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="E31" s="44" t="s">
+      <c r="D32" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="E32" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="37" t="s">
+      <c r="F32" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="G32" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="44"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" s="6" customFormat="1">
-      <c r="A33" s="43">
+      <c r="H32" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1">
+      <c r="A34" s="48">
         <v>25</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D33" s="44" t="s">
+      <c r="B34" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="G34" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I34" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="9"/>
+      <c r="B35" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" s="6" customFormat="1">
+      <c r="A36" s="48">
+        <v>26</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="44" t="s">
+      <c r="D36" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="G33" s="43" t="s">
+      <c r="F36" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="44"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" s="6" customFormat="1">
-      <c r="A35" s="43">
-        <v>26</v>
-      </c>
-      <c r="B35" s="44" t="s">
+      <c r="H36" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I36" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="6" customFormat="1">
+      <c r="A37" s="48">
+        <v>27</v>
+      </c>
+      <c r="B37" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="44" t="s">
+      <c r="C37" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="37" t="s">
+      <c r="F37" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="44"/>
-    </row>
-    <row r="36" spans="1:9" s="6" customFormat="1">
-      <c r="A36" s="43">
-        <v>27</v>
-      </c>
-      <c r="B36" s="44" t="s">
+      <c r="H37" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="I37" s="49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60">
+      <c r="A38" s="29">
+        <v>28</v>
+      </c>
+      <c r="B38" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="44" t="s">
+      <c r="C38" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="G38" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="30"/>
+      <c r="I38" s="37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60">
+      <c r="A39" s="29">
+        <v>29</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="37" t="s">
+      <c r="F39" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="44"/>
-    </row>
-    <row r="37" spans="1:9" ht="60">
-      <c r="A37" s="31">
-        <v>28</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="32" t="s">
+      <c r="H39" s="30"/>
+      <c r="I39" s="37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60">
+      <c r="A40" s="29">
+        <v>30</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="31" t="s">
+      <c r="F40" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="60">
-      <c r="A38" s="31">
-        <v>29</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="32" t="s">
+      <c r="H40" s="30"/>
+      <c r="I40" s="37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="60">
+      <c r="A41" s="29">
+        <v>31</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="31" t="s">
+      <c r="F41" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="60">
-      <c r="A39" s="31">
-        <v>30</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="60">
-      <c r="A40" s="31">
-        <v>31</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="G40" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="39" t="s">
-        <v>239</v>
+      <c r="H41" s="30"/>
+      <c r="I41" s="37" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3114,7 +3204,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H41">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
@@ -3131,7 +3221,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3146,7 +3236,7 @@
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3162,46 +3252,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -3209,49 +3299,49 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -3259,49 +3349,49 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3309,49 +3399,49 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K4" s="40" t="s">
-        <v>234</v>
+        <v>244</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>230</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3359,49 +3449,49 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3409,49 +3499,49 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3459,49 +3549,49 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I7" s="4">
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K7" s="40" t="s">
-        <v>234</v>
+        <v>244</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>230</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3509,49 +3599,49 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K8" s="47" t="s">
-        <v>235</v>
+        <v>244</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>231</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O8" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -3559,49 +3649,49 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I9" s="4">
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>256</v>
+        <v>244</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>247</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="M9" s="40" t="s">
-        <v>255</v>
+        <v>248</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>246</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -3609,49 +3699,49 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I10" s="4">
         <v>1</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -3659,49 +3749,49 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I11" s="4">
         <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -3709,49 +3799,49 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I12" s="4">
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -3759,49 +3849,49 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -3809,49 +3899,49 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="I14" s="4">
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3865,7 +3955,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L1" sqref="L1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3892,34 +3982,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>223</v>
+      <c r="L1" s="40" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -3927,37 +4017,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="H2" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="J2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>225</v>
+      <c r="L2" s="34" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3965,37 +4055,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>224</v>
+        <v>188</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4003,37 +4093,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>224</v>
+        <v>188</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4073,22 +4163,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4096,25 +4186,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4122,25 +4212,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4175,16 +4265,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4192,19 +4282,19 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>219</v>
+        <v>176</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4212,19 +4302,19 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>219</v>
+        <v>176</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4235,10 +4325,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4263,28 +4353,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>233</v>
+      <c r="J1" s="40" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4292,31 +4382,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>234</v>
+        <v>202</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4324,31 +4414,31 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>235</v>
+      <c r="J3" s="44" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4356,28 +4446,51 @@
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3">
+        <v>32</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>189</v>
+      <c r="D5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4391,7 +4504,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4414,22 +4527,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4437,25 +4550,25 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4463,25 +4576,25 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>224</v>
+        <v>267</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4489,16 +4602,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4506,16 +4619,16 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4">
         <v>511111112</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4523,16 +4636,16 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4540,16 +4653,16 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4561,9 +4674,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -4577,9 +4690,10 @@
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4587,48 +4701,54 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="4">
+        <v>123450</v>
+      </c>
+      <c r="E2" s="4">
+        <v>123450</v>
+      </c>
+      <c r="F2" s="4">
+        <v>123451</v>
+      </c>
+      <c r="G2">
+        <v>123451</v>
+      </c>
+      <c r="H2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I2" s="34" t="s">
         <v>261</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="4">
-        <v>123457</v>
-      </c>
-      <c r="G2">
-        <v>123457</v>
-      </c>
-      <c r="H2" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developed Script for Cart & Checkout - Need to debug
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="281">
   <si>
     <t>P_Key</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Mobile</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -729,10 +726,6 @@
     <t>View &amp; Edit Profile Tests</t>
   </si>
   <si>
-    <t>Clarification Logged -  Test Step &amp; Verification is generic, Need Clear Verification Step of What to be verified.
-   Just mentioned to check section &amp; those assertion are not quantifiable &amp; clear.</t>
-  </si>
-  <si>
     <t>ViewAndEditProfile</t>
   </si>
   <si>
@@ -776,9 +769,6 @@
   </si>
   <si>
     <t>MASTER</t>
-  </si>
-  <si>
-    <t>Wallet</t>
   </si>
   <si>
     <t>12</t>
@@ -798,10 +788,6 @@
     - Getting error when used the same number twice, this will cause the script to fail second time. </t>
   </si>
   <si>
-    <t>Clarification Logged
-    - App Issue, Add to cart not Working</t>
-  </si>
-  <si>
     <t>addNewMasterCard</t>
   </si>
   <si>
@@ -843,6 +829,57 @@
   </si>
   <si>
     <t>Automa</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>CartTotal</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>WalletAmount</t>
+  </si>
+  <si>
+    <t>DueWalletAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1035.00 SAR </t>
+  </si>
+  <si>
+    <t>200.00 SAR</t>
+  </si>
+  <si>
+    <t>- -1035.00 SAR</t>
+  </si>
+  <si>
+    <t>30.00 SAR</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1265.00 SAR </t>
+  </si>
+  <si>
+    <t>IOS Not Developed</t>
+  </si>
+  <si>
+    <t>DeliveryCharges</t>
+  </si>
+  <si>
+    <t>DeliveryAddress</t>
+  </si>
+  <si>
+    <t>To : </t>
   </si>
 </sst>
 </file>
@@ -941,7 +978,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -993,6 +1030,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1086,7 +1129,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1154,12 +1197,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1209,13 +1248,148 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1325,22 +1499,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A5:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="WebConfiguration" dataDxfId="11"/>
-    <tableColumn id="2" name="BaseURL" dataDxfId="10"/>
-    <tableColumn id="3" name="Browser" dataDxfId="9"/>
-    <tableColumn id="4" name="Width" dataDxfId="8"/>
-    <tableColumn id="5" name="Height" dataDxfId="7"/>
-    <tableColumn id="6" name="MAXWait" dataDxfId="6"/>
+    <tableColumn id="1" name="WebConfiguration" dataDxfId="29"/>
+    <tableColumn id="2" name="BaseURL" dataDxfId="28"/>
+    <tableColumn id="3" name="Browser" dataDxfId="27"/>
+    <tableColumn id="4" name="Width" dataDxfId="26"/>
+    <tableColumn id="5" name="Height" dataDxfId="25"/>
+    <tableColumn id="6" name="MAXWait" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A13:N19"/>
   <tableColumns count="14">
     <tableColumn id="1" name="MobileConfiguration"/>
@@ -1351,10 +1525,10 @@
     <tableColumn id="6" name="AppName"/>
     <tableColumn id="12" name="AppURL"/>
     <tableColumn id="7" name="AppPackage"/>
-    <tableColumn id="8" name="AppActivity" dataDxfId="4"/>
+    <tableColumn id="8" name="AppActivity" dataDxfId="22"/>
     <tableColumn id="9" name="AppiumURL"/>
     <tableColumn id="10" name="AutomationName"/>
-    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="3"/>
+    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="21"/>
     <tableColumn id="13" name="Project"/>
     <tableColumn id="14" name="Build"/>
   </tableColumns>
@@ -1366,7 +1540,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Platform" dataDxfId="2"/>
+    <tableColumn id="1" name="Platform" dataDxfId="20"/>
     <tableColumn id="2" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1628,7 +1802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1660,10 +1834,10 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
         <v>118</v>
-      </c>
-      <c r="B1" t="s">
-        <v>119</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -1674,10 +1848,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1685,27 +1859,27 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
         <v>123</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>124</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>125</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>126</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>127</v>
-      </c>
-      <c r="F5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1713,27 +1887,27 @@
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>132</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="17">
         <v>1920</v>
@@ -1748,11 +1922,11 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="17">
         <v>1920</v>
@@ -1767,11 +1941,11 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="18">
         <v>1080</v>
@@ -1786,7 +1960,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1797,7 +1971,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1808,46 +1982,46 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
         <v>140</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>141</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>142</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>143</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="G13" t="s">
         <v>145</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>146</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>147</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="K13" t="s">
         <v>149</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>150</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>151</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>152</v>
-      </c>
-      <c r="N13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1855,182 +2029,182 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>155</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>156</v>
-      </c>
-      <c r="E14" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>159</v>
       </c>
       <c r="D15" s="28">
         <v>11</v>
       </c>
       <c r="E15" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" t="s">
         <v>160</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>161</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>162</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="K15" t="s">
         <v>164</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" s="23" t="s">
         <v>165</v>
-      </c>
-      <c r="L15" s="23" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
         <v>167</v>
       </c>
-      <c r="B16" t="s">
-        <v>168</v>
-      </c>
       <c r="C16" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s">
         <v>161</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>162</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="K16" t="s">
         <v>164</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" s="23" t="s">
         <v>165</v>
-      </c>
-      <c r="L16" s="23" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" t="s">
         <v>170</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>172</v>
-      </c>
       <c r="E17" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" t="s">
+        <v>173</v>
+      </c>
+      <c r="H17" t="s">
         <v>161</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="H17" t="s">
-        <v>162</v>
-      </c>
-      <c r="I17" t="s">
-        <v>163</v>
-      </c>
-      <c r="J17" s="26" t="s">
+      <c r="K17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="K17" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="M17" s="22" t="s">
+      <c r="N17" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="N17" s="22" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>178</v>
-      </c>
-      <c r="B18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" t="s">
+        <v>173</v>
+      </c>
+      <c r="H19" t="s">
         <v>161</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
+        <v>162</v>
+      </c>
+      <c r="J19" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="H19" t="s">
-        <v>162</v>
-      </c>
-      <c r="I19" t="s">
-        <v>163</v>
-      </c>
-      <c r="J19" s="26" t="s">
+      <c r="L19" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="L19" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="M19" s="22" t="s">
+      <c r="N19" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2083,28 +2257,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>222</v>
+      <c r="E1" s="38" t="s">
+        <v>221</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2112,31 +2286,31 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>223</v>
+        <v>190</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>222</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J2" s="36" t="s">
         <v>235</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2151,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2163,7 +2337,7 @@
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="43" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
   </cols>
@@ -2200,7 +2374,7 @@
     <row r="2" spans="1:9" s="6" customFormat="1">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2211,94 +2385,94 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="75">
-      <c r="A3" s="46">
+      <c r="A3" s="44">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="46">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="36" t="s">
+      <c r="C4" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="48">
-        <v>2</v>
-      </c>
-      <c r="B4" s="49" t="s">
+      <c r="G4" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="46">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="49" t="s">
+      <c r="C5" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="48">
-        <v>3</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I5" s="49" t="s">
-        <v>259</v>
+      <c r="G5" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2308,361 +2482,345 @@
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="39">
+        <v>5</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30">
-      <c r="A8" s="41">
-        <v>5</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>12</v>
+      <c r="G8" s="46" t="s">
+        <v>264</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30">
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>12</v>
+        <v>53</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="29">
         <v>8</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H11" s="30"/>
-      <c r="I11" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30">
+      <c r="I11" s="35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30">
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30">
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>12</v>
+        <v>57</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30">
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="29">
         <v>12</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>12</v>
+        <v>58</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H15" s="30"/>
-      <c r="I15" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30">
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="29">
         <v>13</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="37" t="s">
-        <v>255</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="I16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="30">
       <c r="A17" s="29">
         <v>14</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30">
+        <v>115</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>12</v>
+        <v>60</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="37" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30">
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="29">
         <v>16</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>12</v>
+        <v>61</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>266</v>
       </c>
       <c r="H19" s="30"/>
-      <c r="I19" s="37" t="s">
-        <v>255</v>
-      </c>
+      <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="9"/>
       <c r="B20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -2673,67 +2831,67 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="48">
+      <c r="A21" s="46">
         <v>17</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I21" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="46">
+        <v>18</v>
+      </c>
+      <c r="B22" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="49" t="s">
+      <c r="C22" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E22" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="50" t="s">
+      <c r="F22" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I21" s="49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="48">
-        <v>18</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I22" s="49" t="s">
-        <v>259</v>
+      <c r="G22" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I22" s="47" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2743,68 +2901,68 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" s="39" customFormat="1" ht="75">
-      <c r="A24" s="48">
+    <row r="24" spans="1:9" s="37" customFormat="1" ht="75">
+      <c r="A24" s="46">
         <v>19</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="37" customFormat="1" ht="60">
+      <c r="A25" s="46">
+        <v>20</v>
+      </c>
+      <c r="B25" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="49" t="s">
+      <c r="C25" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E25" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F25" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I24" s="37" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="39" customFormat="1" ht="60">
-      <c r="A25" s="48">
-        <v>20</v>
-      </c>
-      <c r="B25" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I25" s="37" t="s">
-        <v>264</v>
+      <c r="G25" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2815,38 +2973,38 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="30">
-      <c r="A27" s="48">
+      <c r="A27" s="46">
         <v>21</v>
       </c>
-      <c r="B27" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="52" t="s">
+      <c r="B27" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I27" s="51" t="s">
-        <v>263</v>
+      <c r="G27" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="9"/>
       <c r="B28" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2857,125 +3015,125 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="45">
-      <c r="A29" s="48">
+      <c r="A29" s="46">
         <v>22</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I29" s="35" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45">
+      <c r="A30" s="46">
+        <v>23</v>
+      </c>
+      <c r="B30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="49" t="s">
+      <c r="C30" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="49" t="s">
+      <c r="E30" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F30" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="49" t="s">
+      <c r="G30" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" ht="30">
+      <c r="A31" s="46">
+        <v>24</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="6" customFormat="1" ht="45">
+      <c r="A32" s="46">
+        <v>32</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="I29" s="37" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="45">
-      <c r="A30" s="48">
-        <v>23</v>
-      </c>
-      <c r="B30" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="49" t="s">
+      <c r="E32" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I30" s="37" t="s">
+      <c r="F32" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="G32" s="46" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="6" customFormat="1" ht="30">
-      <c r="A31" s="48">
-        <v>24</v>
-      </c>
-      <c r="B31" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I31" s="49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="6" customFormat="1" ht="45">
-      <c r="A32" s="48">
-        <v>32</v>
-      </c>
-      <c r="B32" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="C32" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="49" t="s">
-        <v>257</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="57" t="s">
-        <v>258</v>
-      </c>
-      <c r="G32" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I32" s="37" t="s">
-        <v>265</v>
+      <c r="H32" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="9"/>
       <c r="B33" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2986,38 +3144,38 @@
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" s="6" customFormat="1">
-      <c r="A34" s="48">
+      <c r="A34" s="46">
         <v>25</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="53" t="s">
+        <v>225</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="C34" s="55" t="s">
-        <v>234</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="55" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I34" s="49" t="s">
-        <v>259</v>
+      <c r="G34" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I34" s="47" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -3028,178 +3186,186 @@
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" s="6" customFormat="1">
-      <c r="A36" s="48">
+      <c r="A36" s="46">
         <v>26</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H36" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I36" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="6" customFormat="1">
+      <c r="A37" s="46">
+        <v>27</v>
+      </c>
+      <c r="B37" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="49" t="s">
+      <c r="C37" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="G36" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I36" s="49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="6" customFormat="1">
-      <c r="A37" s="48">
-        <v>27</v>
-      </c>
-      <c r="B37" s="49" t="s">
+      <c r="F37" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H37" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I37" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="56">
+        <v>28</v>
+      </c>
+      <c r="B38" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="49" t="s">
+      <c r="C38" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="G38" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H38" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="I38" s="59" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="56">
+        <v>29</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="I37" s="49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="60">
-      <c r="A38" s="29">
-        <v>28</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="30" t="s">
+      <c r="F39" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H39" s="57" t="s">
+        <v>265</v>
+      </c>
+      <c r="I39" s="59" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="46">
+        <v>30</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="37" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="60">
-      <c r="A39" s="29">
-        <v>29</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="30" t="s">
+      <c r="F40" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H40" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I40" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="46">
+        <v>31</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="30"/>
-      <c r="I39" s="37" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="60">
-      <c r="A40" s="29">
-        <v>30</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="30"/>
-      <c r="I40" s="37" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="60">
-      <c r="A41" s="29">
-        <v>31</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="30" t="s">
+      <c r="F41" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="37" t="s">
-        <v>233</v>
+      <c r="G41" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I41" s="47" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="53" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3218,10 +3384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3236,15 +3402,20 @@
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:23">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3252,697 +3423,679 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="K1" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="R1" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="S1" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="T1" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="U1" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="W1" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="3">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>187</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="3">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>240</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="3">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K4" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>204</v>
+        <v>242</v>
+      </c>
+      <c r="K4" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>229</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>243</v>
+        <v>199</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>211</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="3">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>188</v>
+        <v>242</v>
+      </c>
+      <c r="K5" s="60" t="s">
+        <v>280</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>240</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="3">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>188</v>
+        <v>242</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>280</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>245</v>
+        <v>187</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>243</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="3">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I7" s="4">
         <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>204</v>
+        <v>242</v>
+      </c>
+      <c r="K7" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>229</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>243</v>
+        <v>199</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>211</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="3">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K8" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>203</v>
+        <v>242</v>
+      </c>
+      <c r="K8" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>230</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="O8" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="3">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I9" s="4">
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="N9" s="36" t="s">
         <v>244</v>
       </c>
-      <c r="K9" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="M9" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="O9" s="4" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>211</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="3">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I10" s="4">
         <v>1</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>188</v>
+        <v>242</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>280</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>249</v>
+        <v>187</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>240</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="T10" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="W10" s="33" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="3">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I11" s="4">
         <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>242</v>
+      </c>
+      <c r="K11" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="3">
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I12" s="4">
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>242</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="3">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>188</v>
+        <v>242</v>
+      </c>
+      <c r="K13" s="60" t="s">
+        <v>280</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>240</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="3">
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="I14" s="4">
         <v>1</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>188</v>
-      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3982,34 +4135,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="L1" s="40" t="s">
-        <v>222</v>
+      <c r="L1" s="38" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4017,37 +4170,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="H2" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="J2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="L2" s="34" t="s">
-        <v>224</v>
+      <c r="L2" s="33" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4055,37 +4208,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L3" s="34" t="s">
-        <v>223</v>
+        <v>187</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4093,37 +4246,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>223</v>
+        <v>187</v>
+      </c>
+      <c r="L4" s="33" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4163,22 +4316,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4186,25 +4339,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4212,25 +4365,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -4244,7 +4397,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4265,16 +4418,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4282,19 +4435,19 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>218</v>
+        <v>175</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4302,19 +4455,19 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>218</v>
+        <v>175</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4353,28 +4506,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>229</v>
+      <c r="J1" s="38" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4382,31 +4535,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>230</v>
+        <v>201</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4414,31 +4567,31 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>231</v>
+      <c r="J3" s="42" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4446,13 +4599,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -4465,32 +4618,32 @@
       <c r="A5" s="3">
         <v>32</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>260</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="J5" s="44" t="s">
-        <v>247</v>
+        <v>201</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4527,22 +4680,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4550,25 +4703,25 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4576,25 +4729,25 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4602,16 +4755,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4619,16 +4772,16 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4">
         <v>511111112</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4636,16 +4789,16 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4653,16 +4806,16 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4701,25 +4854,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>222</v>
+      <c r="I1" s="38" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4727,10 +4880,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>252</v>
+        <v>73</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>249</v>
       </c>
       <c r="D2" s="4">
         <v>123450</v>
@@ -4745,10 +4898,10 @@
         <v>123451</v>
       </c>
       <c r="H2" t="s">
-        <v>239</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>261</v>
+        <v>237</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stability omproved & Time optimised
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="285">
   <si>
     <t>P_Key</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>customerRegistration</t>
-  </si>
-  <si>
-    <t>customerLogintoPIK</t>
   </si>
   <si>
     <t>customerLoginAndLogoutFromPIK</t>
@@ -831,69 +828,80 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>CartTotal</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>WalletAmount</t>
+  </si>
+  <si>
+    <t>DueWalletAmount</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>IOS Not Developed</t>
+  </si>
+  <si>
+    <t>DeliveryCharges</t>
+  </si>
+  <si>
+    <t>DeliveryAddress</t>
+  </si>
+  <si>
+    <t>To :</t>
+  </si>
+  <si>
+    <t>100.00 SAR</t>
+  </si>
+  <si>
+    <t>17.10 SAR</t>
+  </si>
+  <si>
+    <t>14.00 SAR</t>
+  </si>
+  <si>
+    <t>123451</t>
+  </si>
+  <si>
+    <t>Clarification Logged
+- Bug Banner Section Not Displayed</t>
+  </si>
+  <si>
+    <t>customerLoginToPIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-115.00 SAR </t>
+  </si>
+  <si>
+    <t>0.00 SAR</t>
+  </si>
+  <si>
+    <t>131.10 SAR</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>CartTotal</t>
-  </si>
-  <si>
-    <t>VAT</t>
-  </si>
-  <si>
-    <t>WalletAmount</t>
-  </si>
-  <si>
-    <t>DueWalletAmount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1035.00 SAR </t>
-  </si>
-  <si>
-    <t>- -1035.00 SAR</t>
-  </si>
-  <si>
-    <t>TotalAmount</t>
-  </si>
-  <si>
-    <t>IOS Not Developed</t>
-  </si>
-  <si>
-    <t>DeliveryCharges</t>
-  </si>
-  <si>
-    <t>DeliveryAddress</t>
-  </si>
-  <si>
-    <t>To :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarification Logged
-  - Need User with Wallet Amount </t>
-  </si>
-  <si>
-    <t>100.00 SAR</t>
-  </si>
-  <si>
-    <t>17.10 SAR</t>
-  </si>
-  <si>
-    <t>14.00 SAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">131.10 SAR </t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>Failed</t>
+    <t>Completed 
+- Note Ensure User has Wallet Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <numFmts count="0"/>
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,6 +991,17 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1240,22 +1259,160 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="35">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1377,22 +1534,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table20" displayName="Table20" ref="A5:F11" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A5:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="WebConfiguration" dataDxfId="12"/>
-    <tableColumn id="2" name="BaseURL" dataDxfId="11"/>
-    <tableColumn id="3" name="Browser" dataDxfId="10"/>
-    <tableColumn id="4" name="Width" dataDxfId="9"/>
-    <tableColumn id="5" name="Height" dataDxfId="8"/>
-    <tableColumn id="6" name="MAXWait" dataDxfId="7"/>
+    <tableColumn id="1" name="WebConfiguration" dataDxfId="32"/>
+    <tableColumn id="2" name="BaseURL" dataDxfId="31"/>
+    <tableColumn id="3" name="Browser" dataDxfId="30"/>
+    <tableColumn id="4" name="Width" dataDxfId="29"/>
+    <tableColumn id="5" name="Height" dataDxfId="28"/>
+    <tableColumn id="6" name="MAXWait" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table21" displayName="Table21" ref="A13:N19" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A13:N19"/>
   <tableColumns count="14">
     <tableColumn id="1" name="MobileConfiguration"/>
@@ -1403,10 +1560,10 @@
     <tableColumn id="6" name="AppName"/>
     <tableColumn id="12" name="AppURL"/>
     <tableColumn id="7" name="AppPackage"/>
-    <tableColumn id="8" name="AppActivity" dataDxfId="5"/>
+    <tableColumn id="8" name="AppActivity" dataDxfId="25"/>
     <tableColumn id="9" name="AppiumURL"/>
     <tableColumn id="10" name="AutomationName"/>
-    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="4"/>
+    <tableColumn id="11" name="AutoGrantPermissions" dataDxfId="24"/>
     <tableColumn id="13" name="Project"/>
     <tableColumn id="14" name="Build"/>
   </tableColumns>
@@ -1418,7 +1575,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1923" displayName="Table1923" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Platform" dataDxfId="3"/>
+    <tableColumn id="1" name="Platform" dataDxfId="23"/>
     <tableColumn id="2" name="Reference"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1680,7 +1837,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1696,26 +1853,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
         <v>117</v>
-      </c>
-      <c r="B1" t="s">
-        <v>118</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -1726,10 +1883,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1737,27 +1894,27 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>122</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>123</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>124</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>125</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>126</v>
-      </c>
-      <c r="F5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1765,27 +1922,27 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>131</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="15">
         <v>1920</v>
@@ -1800,11 +1957,11 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" s="15">
         <v>1920</v>
@@ -1819,11 +1976,11 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9" s="16">
         <v>1080</v>
@@ -1838,7 +1995,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1849,7 +2006,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -1860,46 +2017,46 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" t="s">
         <v>139</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>140</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>141</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>142</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" t="s">
         <v>144</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>145</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>146</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="K13" t="s">
         <v>148</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>149</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>150</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>151</v>
-      </c>
-      <c r="N13" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1907,182 +2064,182 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
         <v>153</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>154</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>155</v>
-      </c>
-      <c r="E14" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>157</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>158</v>
       </c>
       <c r="D15" s="26">
         <v>11</v>
       </c>
       <c r="E15" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" t="s">
         <v>159</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>160</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>161</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="K15" t="s">
         <v>163</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" t="s">
         <v>166</v>
       </c>
-      <c r="B16" t="s">
-        <v>167</v>
-      </c>
       <c r="C16" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" t="s">
         <v>160</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>161</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="K16" t="s">
         <v>163</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s">
         <v>169</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>171</v>
-      </c>
       <c r="E17" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H17" t="s">
         <v>160</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
+        <v>161</v>
+      </c>
+      <c r="J17" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="H17" t="s">
-        <v>161</v>
-      </c>
-      <c r="I17" t="s">
-        <v>162</v>
-      </c>
-      <c r="J17" s="24" t="s">
+      <c r="K17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="M17" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="K17" t="s">
-        <v>164</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="M17" s="20" t="s">
+      <c r="N17" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="25" t="s">
         <v>177</v>
-      </c>
-      <c r="B18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>248</v>
-      </c>
       <c r="F19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" t="s">
         <v>160</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
+        <v>161</v>
+      </c>
+      <c r="J19" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="H19" t="s">
-        <v>161</v>
-      </c>
-      <c r="I19" t="s">
-        <v>162</v>
-      </c>
-      <c r="J19" s="24" t="s">
+      <c r="L19" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="M19" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="L19" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="M19" s="20" t="s">
+      <c r="N19" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="N19" s="20" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2110,21 +2267,21 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2135,28 +2292,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2164,31 +2321,31 @@
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2203,21 +2360,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="55.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="12" width="8.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="55.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2270,25 +2427,25 @@
         <v>17</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H3" s="31" t="s">
         <v>282</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2296,28 +2453,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H4" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2325,28 +2482,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H5" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2358,7 +2515,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="11"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="8"/>
     </row>
@@ -2367,28 +2524,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H7" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I7" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2396,28 +2553,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="H8" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I8" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2425,28 +2582,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H9" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I9" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2454,28 +2611,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H10" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I10" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2483,26 +2640,26 @@
         <v>8</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="32" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2510,28 +2667,28 @@
         <v>9</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H12" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2539,28 +2696,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2568,28 +2725,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="42" t="s">
-        <v>30</v>
-      </c>
       <c r="D14" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
@@ -2597,28 +2754,28 @@
         <v>12</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H15" s="42" t="s">
-        <v>282</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>276</v>
+        <v>281</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2626,28 +2783,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
@@ -2655,28 +2812,28 @@
         <v>14</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H17" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2684,28 +2841,28 @@
         <v>15</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H18" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2713,28 +2870,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H19" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2746,7 +2903,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="11"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="9"/>
       <c r="I20" s="8"/>
     </row>
@@ -2755,28 +2912,28 @@
         <v>17</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H21" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2784,40 +2941,40 @@
         <v>18</v>
       </c>
       <c r="B22" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="42" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H22" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I22" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="8"/>
       <c r="B23" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="8"/>
     </row>
@@ -2826,28 +2983,28 @@
         <v>19</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H24" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="34" customFormat="1" ht="60">
@@ -2855,40 +3012,40 @@
         <v>20</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H25" s="42" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="8"/>
       <c r="B26" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="11"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="8"/>
     </row>
@@ -2897,28 +3054,28 @@
         <v>21</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I27" s="44" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2930,7 +3087,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="11"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="8"/>
     </row>
@@ -2939,28 +3096,28 @@
         <v>22</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H29" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45">
@@ -2968,28 +3125,28 @@
         <v>23</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E30" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H30" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" ht="30">
@@ -2997,28 +3154,28 @@
         <v>24</v>
       </c>
       <c r="B31" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="49" t="s">
-        <v>39</v>
-      </c>
       <c r="D31" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E31" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H31" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I31" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1" ht="45">
@@ -3026,40 +3183,40 @@
         <v>32</v>
       </c>
       <c r="B32" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="42" t="s">
         <v>251</v>
-      </c>
-      <c r="C32" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>252</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H32" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="8"/>
       <c r="B33" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="11"/>
+      <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="8"/>
     </row>
@@ -3068,40 +3225,40 @@
         <v>25</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H34" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I34" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="11"/>
+      <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="8"/>
     </row>
@@ -3110,28 +3267,28 @@
         <v>26</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="42" t="s">
         <v>75</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>76</v>
       </c>
       <c r="E36" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H36" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I36" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="5" customFormat="1">
@@ -3139,86 +3296,86 @@
         <v>27</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H37" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I37" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="51">
+      <c r="A38" s="41">
         <v>28</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="H38" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="I38" s="42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30">
+      <c r="A39" s="53">
+        <v>29</v>
+      </c>
+      <c r="B39" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="52" t="s">
+      <c r="C39" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E39" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="H38" s="52" t="s">
+      <c r="F39" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="H39" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="I38" s="54" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="51">
-        <v>29</v>
-      </c>
-      <c r="B39" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G39" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="H39" s="52" t="s">
-        <v>282</v>
-      </c>
-      <c r="I39" s="54" t="s">
-        <v>254</v>
+      <c r="I39" s="32" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3226,28 +3383,28 @@
         <v>30</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H40" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I40" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3255,47 +3412,82 @@
         <v>31</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>11</v>
       </c>
       <c r="F41" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H41" s="42" t="s">
         <v>281</v>
       </c>
       <c r="I41" s="42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="54" operator="equal">
+  <conditionalFormatting sqref="G1:G19 G21:G1048576">
+    <cfRule type="cellIs" dxfId="22" priority="61" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G33">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:H41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21:G41 H3:H41 G3:G19">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
@@ -3311,35 +3503,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3350,67 +3542,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>197</v>
-      </c>
       <c r="R1" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="S1" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="U1" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="V1" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="W1" s="35" t="s">
         <v>267</v>
-      </c>
-      <c r="S1" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>268</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>273</v>
-      </c>
-      <c r="V1" s="35" t="s">
-        <v>266</v>
-      </c>
-      <c r="W1" s="35" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -3418,31 +3610,31 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I2" s="3">
         <v>2</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -3457,40 +3649,40 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E3" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -3502,52 +3694,52 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D4" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K4" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K4" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -3555,40 +3747,40 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D5" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E5" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K5" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K5" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -3600,40 +3792,40 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D6" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K6" s="52" t="s">
+        <v>271</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="K6" s="55" t="s">
-        <v>275</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -3645,52 +3837,52 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D7" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E7" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K7" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K7" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -3698,52 +3890,52 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D8" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D8" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E8" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K8" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K8" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L8" s="38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P8" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -3751,52 +3943,52 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D9" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K9" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K9" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L9" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="N9" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -3804,70 +3996,70 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>190</v>
+        <v>61</v>
+      </c>
+      <c r="C10" s="3">
+        <v>566666666</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>189</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I10" s="3">
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K10" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K10" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R10" s="38" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="S10" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="T10" s="38" t="s">
-        <v>270</v>
+        <v>272</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="U10" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="V10" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="W10" s="30" t="s">
         <v>279</v>
-      </c>
-      <c r="V10" s="38" t="s">
-        <v>278</v>
-      </c>
-      <c r="W10" s="30" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -3875,67 +4067,67 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D11" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K11" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K11" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U11" s="38" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="V11" s="38" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="W11" s="30" t="s">
         <v>280</v>
@@ -3946,40 +4138,40 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D12" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E12" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K12" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K12" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -3991,40 +4183,40 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D13" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="K13" s="55" t="s">
-        <v>275</v>
+        <v>241</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>271</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -4036,25 +4228,25 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D14" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E14" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
@@ -4079,23 +4271,23 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4106,34 +4298,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>186</v>
-      </c>
       <c r="L1" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4144,34 +4336,34 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="H2" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="J2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="L2" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4179,37 +4371,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>275</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4217,37 +4409,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>275</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4264,19 +4456,19 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4287,22 +4479,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4310,25 +4502,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4336,25 +4528,25 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E3" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4365,20 +4557,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4389,16 +4581,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4406,19 +4598,19 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4426,19 +4618,19 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4452,21 +4644,21 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4477,28 +4669,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>197</v>
-      </c>
       <c r="J1" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4506,31 +4698,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4538,31 +4730,31 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="J3" s="38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -4570,13 +4762,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>190</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>275</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -4590,31 +4782,31 @@
         <v>32</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D5" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E5" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5" s="38" t="s">
         <v>244</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="J5" s="38" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4628,19 +4820,19 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4651,22 +4843,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4674,25 +4866,25 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4700,25 +4892,25 @@
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4726,16 +4918,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D4" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4743,16 +4935,16 @@
         <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="3">
-        <v>511111112</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D5" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4760,16 +4952,16 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D6" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4777,16 +4969,16 @@
         <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="D7" s="33" t="s">
+        <v>275</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4801,20 +4993,20 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4825,25 +5017,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G1" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>186</v>
-      </c>
       <c r="I1" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4851,28 +5043,28 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" s="3">
-        <v>123451</v>
+        <v>123452</v>
       </c>
       <c r="E2" s="3">
-        <v>123451</v>
+        <v>123452</v>
       </c>
       <c r="F2" s="3">
-        <v>123452</v>
+        <v>123453</v>
       </c>
       <c r="G2">
-        <v>123452</v>
+        <v>123453</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>